<commit_message>
new data, change years, no data as fill variable
</commit_message>
<xml_diff>
--- a/data/Enforcement_Policies_Data.xlsx
+++ b/data/Enforcement_Policies_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhou/Documents/Projects/state-immigration/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmelgar/Desktop/urban-institute/projects/2021/20211102-state-immigration-policy/state-immigration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13419352-A4AE-7E49-BC10-BCC331152241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15600" tabRatio="758" activeTab="5"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="35700" windowHeight="17760" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="287(g) Policies" sheetId="4" r:id="rId1"/>
@@ -29,10 +30,19 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'287(g) Policies'!$A$1:$AT$108</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'287(g) Policies'!$A:$BD</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2274,7 +2284,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3082,6 +3092,45 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3095,45 +3144,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3217,87 +3227,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3316,6 +3245,87 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3333,13 +3343,16 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3631,16 +3644,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AT119"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3689,132 +3702,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A1" s="205" t="s">
+      <c r="A1" s="191" t="s">
         <v>341</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
-      <c r="F1" s="205"/>
-      <c r="G1" s="205"/>
-      <c r="H1" s="205"/>
-      <c r="I1" s="205"/>
-      <c r="J1" s="205"/>
-      <c r="K1" s="205"/>
-      <c r="L1" s="205"/>
-      <c r="M1" s="205"/>
-      <c r="N1" s="205"/>
-      <c r="O1" s="205"/>
-      <c r="P1" s="205"/>
-      <c r="Q1" s="205"/>
-      <c r="R1" s="205"/>
-      <c r="S1" s="205"/>
-      <c r="T1" s="205"/>
-      <c r="U1" s="205"/>
-      <c r="V1" s="205"/>
-      <c r="W1" s="205"/>
-      <c r="X1" s="205"/>
-      <c r="Y1" s="205"/>
-      <c r="Z1" s="205"/>
-      <c r="AA1" s="205"/>
-      <c r="AB1" s="205"/>
-      <c r="AC1" s="205"/>
-      <c r="AD1" s="205"/>
-      <c r="AE1" s="205"/>
-      <c r="AF1" s="205"/>
-      <c r="AG1" s="205"/>
-      <c r="AH1" s="205"/>
-      <c r="AI1" s="205"/>
-      <c r="AJ1" s="205"/>
-      <c r="AK1" s="205"/>
-      <c r="AL1" s="205"/>
-      <c r="AM1" s="205"/>
-      <c r="AN1" s="205"/>
-      <c r="AO1" s="205"/>
-      <c r="AP1" s="205"/>
-      <c r="AQ1" s="205"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="191"/>
+      <c r="P1" s="191"/>
+      <c r="Q1" s="191"/>
+      <c r="R1" s="191"/>
+      <c r="S1" s="191"/>
+      <c r="T1" s="191"/>
+      <c r="U1" s="191"/>
+      <c r="V1" s="191"/>
+      <c r="W1" s="191"/>
+      <c r="X1" s="191"/>
+      <c r="Y1" s="191"/>
+      <c r="Z1" s="191"/>
+      <c r="AA1" s="191"/>
+      <c r="AB1" s="191"/>
+      <c r="AC1" s="191"/>
+      <c r="AD1" s="191"/>
+      <c r="AE1" s="191"/>
+      <c r="AF1" s="191"/>
+      <c r="AG1" s="191"/>
+      <c r="AH1" s="191"/>
+      <c r="AI1" s="191"/>
+      <c r="AJ1" s="191"/>
+      <c r="AK1" s="191"/>
+      <c r="AL1" s="191"/>
+      <c r="AM1" s="191"/>
+      <c r="AN1" s="191"/>
+      <c r="AO1" s="191"/>
+      <c r="AP1" s="191"/>
+      <c r="AQ1" s="191"/>
     </row>
     <row r="2" spans="1:46" s="65" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="197"/>
-      <c r="B2" s="193">
+      <c r="A2" s="189"/>
+      <c r="B2" s="194">
         <v>2002</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193">
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="194">
         <v>2003</v>
       </c>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193">
+      <c r="F2" s="194"/>
+      <c r="G2" s="194"/>
+      <c r="H2" s="194">
         <v>2004</v>
       </c>
-      <c r="I2" s="193"/>
-      <c r="J2" s="193"/>
-      <c r="K2" s="193">
+      <c r="I2" s="194"/>
+      <c r="J2" s="194"/>
+      <c r="K2" s="194">
         <v>2005</v>
       </c>
-      <c r="L2" s="193"/>
-      <c r="M2" s="193"/>
-      <c r="N2" s="193">
+      <c r="L2" s="194"/>
+      <c r="M2" s="194"/>
+      <c r="N2" s="194">
         <v>2006</v>
       </c>
-      <c r="O2" s="193"/>
-      <c r="P2" s="193"/>
-      <c r="Q2" s="193">
+      <c r="O2" s="194"/>
+      <c r="P2" s="194"/>
+      <c r="Q2" s="194">
         <v>2007</v>
       </c>
-      <c r="R2" s="193"/>
-      <c r="S2" s="193"/>
-      <c r="T2" s="193">
+      <c r="R2" s="194"/>
+      <c r="S2" s="194"/>
+      <c r="T2" s="194">
         <v>2008</v>
       </c>
-      <c r="U2" s="193"/>
-      <c r="V2" s="193"/>
-      <c r="W2" s="193">
+      <c r="U2" s="194"/>
+      <c r="V2" s="194"/>
+      <c r="W2" s="194">
         <v>2009</v>
       </c>
-      <c r="X2" s="193"/>
-      <c r="Y2" s="193"/>
-      <c r="Z2" s="193">
+      <c r="X2" s="194"/>
+      <c r="Y2" s="194"/>
+      <c r="Z2" s="194">
         <v>2010</v>
       </c>
-      <c r="AA2" s="193"/>
-      <c r="AB2" s="193"/>
-      <c r="AC2" s="193">
+      <c r="AA2" s="194"/>
+      <c r="AB2" s="194"/>
+      <c r="AC2" s="194">
         <v>2011</v>
       </c>
-      <c r="AD2" s="193"/>
-      <c r="AE2" s="193"/>
-      <c r="AF2" s="193">
+      <c r="AD2" s="194"/>
+      <c r="AE2" s="194"/>
+      <c r="AF2" s="194">
         <v>2012</v>
       </c>
-      <c r="AG2" s="193"/>
-      <c r="AH2" s="193"/>
-      <c r="AI2" s="193">
+      <c r="AG2" s="194"/>
+      <c r="AH2" s="194"/>
+      <c r="AI2" s="194">
         <v>2013</v>
       </c>
-      <c r="AJ2" s="193"/>
-      <c r="AK2" s="193"/>
-      <c r="AL2" s="193">
+      <c r="AJ2" s="194"/>
+      <c r="AK2" s="194"/>
+      <c r="AL2" s="194">
         <v>2014</v>
       </c>
-      <c r="AM2" s="193"/>
-      <c r="AN2" s="193"/>
-      <c r="AO2" s="193">
+      <c r="AM2" s="194"/>
+      <c r="AN2" s="194"/>
+      <c r="AO2" s="194">
         <v>2015</v>
       </c>
-      <c r="AP2" s="193"/>
-      <c r="AQ2" s="193"/>
-      <c r="AR2" s="193">
+      <c r="AP2" s="194"/>
+      <c r="AQ2" s="194"/>
+      <c r="AR2" s="194">
         <v>2016</v>
       </c>
-      <c r="AS2" s="193"/>
-      <c r="AT2" s="193"/>
-    </row>
-    <row r="3" spans="1:46" s="56" customFormat="1" ht="26" x14ac:dyDescent="0.15">
-      <c r="A3" s="198"/>
+      <c r="AS2" s="194"/>
+      <c r="AT2" s="194"/>
+    </row>
+    <row r="3" spans="1:46" s="56" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A3" s="190"/>
       <c r="B3" s="63" t="s">
         <v>81</v>
       </c>
@@ -3952,7 +3965,7 @@
       </c>
     </row>
     <row r="4" spans="1:46" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="199" t="s">
+      <c r="A4" s="192" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="7"/>
@@ -4085,8 +4098,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="201"/>
+    <row r="5" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A5" s="193"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
@@ -4157,7 +4170,7 @@
       <c r="AS5" s="2"/>
       <c r="AT5" s="3"/>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="59" t="s">
         <v>1</v>
       </c>
@@ -4203,8 +4216,8 @@
       <c r="AS6" s="5"/>
       <c r="AT6" s="6"/>
     </row>
-    <row r="7" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A7" s="199" t="s">
+    <row r="7" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A7" s="192" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7"/>
@@ -4325,8 +4338,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A8" s="200"/>
+    <row r="8" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A8" s="198"/>
       <c r="B8" s="42"/>
       <c r="C8" s="32"/>
       <c r="D8" s="33"/>
@@ -4433,8 +4446,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A9" s="200"/>
+    <row r="9" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A9" s="198"/>
       <c r="B9" s="42"/>
       <c r="C9" s="32"/>
       <c r="D9" s="33"/>
@@ -4541,8 +4554,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A10" s="200"/>
+    <row r="10" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A10" s="198"/>
       <c r="B10" s="42"/>
       <c r="C10" s="32"/>
       <c r="D10" s="33"/>
@@ -4641,8 +4654,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="200"/>
+    <row r="11" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A11" s="198"/>
       <c r="B11" s="42"/>
       <c r="C11" s="32"/>
       <c r="D11" s="33"/>
@@ -4706,8 +4719,8 @@
       <c r="AS11" s="32"/>
       <c r="AT11" s="33"/>
     </row>
-    <row r="12" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A12" s="200"/>
+    <row r="12" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A12" s="198"/>
       <c r="B12" s="42"/>
       <c r="C12" s="32"/>
       <c r="D12" s="33"/>
@@ -4772,8 +4785,8 @@
       <c r="AS12" s="32"/>
       <c r="AT12" s="33"/>
     </row>
-    <row r="13" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" s="200"/>
+    <row r="13" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A13" s="198"/>
       <c r="B13" s="42"/>
       <c r="C13" s="32"/>
       <c r="D13" s="33"/>
@@ -4838,8 +4851,8 @@
       <c r="AS13" s="32"/>
       <c r="AT13" s="33"/>
     </row>
-    <row r="14" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A14" s="200"/>
+    <row r="14" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A14" s="198"/>
       <c r="B14" s="42"/>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
@@ -4896,8 +4909,8 @@
       <c r="AS14" s="32"/>
       <c r="AT14" s="33"/>
     </row>
-    <row r="15" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A15" s="200"/>
+    <row r="15" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" s="198"/>
       <c r="B15" s="42"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
@@ -4954,8 +4967,8 @@
       <c r="AS15" s="32"/>
       <c r="AT15" s="33"/>
     </row>
-    <row r="16" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A16" s="200"/>
+    <row r="16" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A16" s="198"/>
       <c r="B16" s="42"/>
       <c r="C16" s="32"/>
       <c r="D16" s="33"/>
@@ -5005,8 +5018,8 @@
       <c r="AS16" s="2"/>
       <c r="AT16" s="3"/>
     </row>
-    <row r="17" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A17" s="199" t="s">
+    <row r="17" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A17" s="192" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="7"/>
@@ -5115,8 +5128,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A18" s="200"/>
+    <row r="18" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A18" s="198"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
@@ -5223,8 +5236,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A19" s="200"/>
+    <row r="19" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A19" s="198"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
       <c r="D19" s="33"/>
@@ -5303,8 +5316,8 @@
       <c r="AS19" s="32"/>
       <c r="AT19" s="33"/>
     </row>
-    <row r="20" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A20" s="201"/>
+    <row r="20" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A20" s="193"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
@@ -5386,8 +5399,8 @@
       <c r="AS20" s="2"/>
       <c r="AT20" s="3"/>
     </row>
-    <row r="21" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A21" s="199" t="s">
+    <row r="21" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A21" s="192" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="7"/>
@@ -5508,8 +5521,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A22" s="200"/>
+    <row r="22" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A22" s="198"/>
       <c r="B22" s="42"/>
       <c r="C22" s="32"/>
       <c r="D22" s="33"/>
@@ -5622,8 +5635,8 @@
       <c r="AS22" s="32"/>
       <c r="AT22" s="33"/>
     </row>
-    <row r="23" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A23" s="200"/>
+    <row r="23" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="198"/>
       <c r="B23" s="42"/>
       <c r="C23" s="32"/>
       <c r="D23" s="33"/>
@@ -5707,8 +5720,8 @@
       <c r="AS23" s="32"/>
       <c r="AT23" s="33"/>
     </row>
-    <row r="24" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A24" s="201"/>
+    <row r="24" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A24" s="193"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
@@ -5797,8 +5810,8 @@
       <c r="AS24" s="2"/>
       <c r="AT24" s="3"/>
     </row>
-    <row r="25" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A25" s="199" t="s">
+    <row r="25" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A25" s="192" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="7"/>
@@ -5895,8 +5908,8 @@
       <c r="AS25" s="8"/>
       <c r="AT25" s="9"/>
     </row>
-    <row r="26" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A26" s="201"/>
+    <row r="26" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A26" s="193"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
@@ -5979,7 +5992,7 @@
       <c r="AS26" s="2"/>
       <c r="AT26" s="3"/>
     </row>
-    <row r="27" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="57" t="s">
         <v>6</v>
       </c>
@@ -6053,7 +6066,7 @@
       <c r="AS27" s="5"/>
       <c r="AT27" s="6"/>
     </row>
-    <row r="28" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" s="57" t="s">
         <v>7</v>
       </c>
@@ -6121,7 +6134,7 @@
       <c r="AS28" s="5"/>
       <c r="AT28" s="6"/>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="59" t="s">
         <v>234</v>
       </c>
@@ -6171,8 +6184,8 @@
       <c r="AS29" s="5"/>
       <c r="AT29" s="6"/>
     </row>
-    <row r="30" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A30" s="202" t="s">
+    <row r="30" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A30" s="195" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="39">
@@ -6311,8 +6324,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A31" s="204"/>
+    <row r="31" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A31" s="197"/>
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
       <c r="D31" s="33"/>
@@ -6419,8 +6432,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A32" s="204"/>
+    <row r="32" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A32" s="197"/>
       <c r="B32" s="42"/>
       <c r="C32" s="32"/>
       <c r="D32" s="33"/>
@@ -6491,8 +6504,8 @@
       <c r="AS32" s="32"/>
       <c r="AT32" s="33"/>
     </row>
-    <row r="33" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A33" s="204"/>
+    <row r="33" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A33" s="197"/>
       <c r="B33" s="42"/>
       <c r="C33" s="32"/>
       <c r="D33" s="33"/>
@@ -6563,8 +6576,8 @@
       <c r="AS33" s="32"/>
       <c r="AT33" s="33"/>
     </row>
-    <row r="34" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A34" s="204"/>
+    <row r="34" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A34" s="197"/>
       <c r="B34" s="42"/>
       <c r="C34" s="32"/>
       <c r="D34" s="33"/>
@@ -6613,8 +6626,8 @@
       <c r="AS34" s="32"/>
       <c r="AT34" s="33"/>
     </row>
-    <row r="35" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A35" s="204"/>
+    <row r="35" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A35" s="197"/>
       <c r="B35" s="42"/>
       <c r="C35" s="32"/>
       <c r="D35" s="33"/>
@@ -6664,7 +6677,7 @@
       <c r="AT35" s="33"/>
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A36" s="203"/>
+      <c r="A36" s="196"/>
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
@@ -6705,8 +6718,8 @@
       <c r="AS36" s="2"/>
       <c r="AT36" s="3"/>
     </row>
-    <row r="37" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A37" s="202" t="s">
+    <row r="37" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A37" s="195" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="7"/>
@@ -6815,8 +6828,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A38" s="204"/>
+    <row r="38" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A38" s="197"/>
       <c r="B38" s="42"/>
       <c r="C38" s="32"/>
       <c r="D38" s="33"/>
@@ -6923,8 +6936,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A39" s="204"/>
+    <row r="39" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A39" s="197"/>
       <c r="B39" s="42"/>
       <c r="C39" s="32"/>
       <c r="D39" s="33"/>
@@ -7024,8 +7037,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A40" s="204"/>
+    <row r="40" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A40" s="197"/>
       <c r="B40" s="42"/>
       <c r="C40" s="32"/>
       <c r="D40" s="33"/>
@@ -7125,8 +7138,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A41" s="203"/>
+    <row r="41" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A41" s="196"/>
       <c r="B41" s="1"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
@@ -7197,7 +7210,7 @@
       <c r="AS41" s="2"/>
       <c r="AT41" s="3"/>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="58" t="s">
         <v>10</v>
       </c>
@@ -7247,7 +7260,7 @@
       <c r="AS42" s="5"/>
       <c r="AT42" s="6"/>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="58" t="s">
         <v>11</v>
       </c>
@@ -7297,7 +7310,7 @@
       <c r="AS43" s="5"/>
       <c r="AT43" s="6"/>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="58" t="s">
         <v>12</v>
       </c>
@@ -7347,7 +7360,7 @@
       <c r="AS44" s="5"/>
       <c r="AT44" s="6"/>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="58" t="s">
         <v>13</v>
       </c>
@@ -7397,7 +7410,7 @@
       <c r="AS45" s="5"/>
       <c r="AT45" s="6"/>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
@@ -7447,7 +7460,7 @@
       <c r="AS46" s="5"/>
       <c r="AT46" s="6"/>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="58" t="s">
         <v>15</v>
       </c>
@@ -7497,7 +7510,7 @@
       <c r="AS47" s="5"/>
       <c r="AT47" s="6"/>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="58" t="s">
         <v>16</v>
       </c>
@@ -7547,7 +7560,7 @@
       <c r="AS48" s="5"/>
       <c r="AT48" s="6"/>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="58" t="s">
         <v>17</v>
       </c>
@@ -7597,7 +7610,7 @@
       <c r="AS49" s="5"/>
       <c r="AT49" s="6"/>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="58" t="s">
         <v>18</v>
       </c>
@@ -7647,8 +7660,8 @@
       <c r="AS50" s="8"/>
       <c r="AT50" s="9"/>
     </row>
-    <row r="51" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A51" s="194" t="s">
+    <row r="51" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A51" s="199" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="39"/>
@@ -7751,8 +7764,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A52" s="195"/>
+    <row r="52" spans="1:46" ht="14" x14ac:dyDescent="0.15">
+      <c r="A52" s="200"/>
       <c r="B52" s="36"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
@@ -7805,8 +7818,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A53" s="196" t="s">
+    <row r="53" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A53" s="188" t="s">
         <v>20</v>
       </c>
       <c r="B53" s="7"/>
@@ -7915,8 +7928,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A54" s="197"/>
+    <row r="54" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A54" s="189"/>
       <c r="B54" s="42"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
@@ -7974,8 +7987,8 @@
       <c r="AS54" s="32"/>
       <c r="AT54" s="33"/>
     </row>
-    <row r="55" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A55" s="198"/>
+    <row r="55" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A55" s="190"/>
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
@@ -8036,7 +8049,7 @@
       <c r="AS55" s="2"/>
       <c r="AT55" s="3"/>
     </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="58" t="s">
         <v>48</v>
       </c>
@@ -8086,7 +8099,7 @@
       <c r="AS56" s="5"/>
       <c r="AT56" s="6"/>
     </row>
-    <row r="57" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" s="58" t="s">
         <v>21</v>
       </c>
@@ -8160,7 +8173,7 @@
       <c r="AS57" s="5"/>
       <c r="AT57" s="6"/>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="58" t="s">
         <v>22</v>
       </c>
@@ -8210,7 +8223,7 @@
       <c r="AS58" s="5"/>
       <c r="AT58" s="6"/>
     </row>
-    <row r="59" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A59" s="58" t="s">
         <v>23</v>
       </c>
@@ -8284,7 +8297,7 @@
       <c r="AS59" s="5"/>
       <c r="AT59" s="6"/>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="58" t="s">
         <v>24</v>
       </c>
@@ -8334,7 +8347,7 @@
       <c r="AS60" s="5"/>
       <c r="AT60" s="6"/>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="58" t="s">
         <v>25</v>
       </c>
@@ -8384,7 +8397,7 @@
       <c r="AS61" s="5"/>
       <c r="AT61" s="6"/>
     </row>
-    <row r="62" spans="1:46" ht="39" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:46" ht="42" x14ac:dyDescent="0.15">
       <c r="A62" s="58" t="s">
         <v>26</v>
       </c>
@@ -8488,7 +8501,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A63" s="58" t="s">
         <v>27</v>
       </c>
@@ -8562,8 +8575,8 @@
       <c r="AS63" s="5"/>
       <c r="AT63" s="6"/>
     </row>
-    <row r="64" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A64" s="196" t="s">
+    <row r="64" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A64" s="188" t="s">
         <v>28</v>
       </c>
       <c r="B64" s="35"/>
@@ -8666,8 +8679,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A65" s="197"/>
+    <row r="65" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A65" s="189"/>
       <c r="B65" s="34"/>
       <c r="C65" s="32"/>
       <c r="D65" s="33"/>
@@ -8760,8 +8773,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A66" s="198"/>
+    <row r="66" spans="1:46" ht="14" x14ac:dyDescent="0.15">
+      <c r="A66" s="190"/>
       <c r="B66" s="37"/>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
@@ -8814,7 +8827,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A67" s="58" t="s">
         <v>29</v>
       </c>
@@ -8900,7 +8913,7 @@
       <c r="AS67" s="2"/>
       <c r="AT67" s="3"/>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="58" t="s">
         <v>30</v>
       </c>
@@ -8950,8 +8963,8 @@
       <c r="AS68" s="5"/>
       <c r="AT68" s="6"/>
     </row>
-    <row r="69" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A69" s="202" t="s">
+    <row r="69" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A69" s="195" t="s">
         <v>31</v>
       </c>
       <c r="B69" s="7"/>
@@ -9066,8 +9079,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A70" s="204"/>
+    <row r="70" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A70" s="197"/>
       <c r="B70" s="42"/>
       <c r="C70" s="32"/>
       <c r="D70" s="33"/>
@@ -9174,8 +9187,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A71" s="204"/>
+    <row r="71" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A71" s="197"/>
       <c r="B71" s="42"/>
       <c r="C71" s="32"/>
       <c r="D71" s="33"/>
@@ -9282,8 +9295,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A72" s="204"/>
+    <row r="72" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A72" s="197"/>
       <c r="B72" s="42"/>
       <c r="C72" s="32"/>
       <c r="D72" s="33"/>
@@ -9390,8 +9403,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A73" s="204"/>
+    <row r="73" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A73" s="197"/>
       <c r="B73" s="42"/>
       <c r="C73" s="32"/>
       <c r="D73" s="33"/>
@@ -9491,8 +9504,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A74" s="204"/>
+    <row r="74" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A74" s="197"/>
       <c r="B74" s="42"/>
       <c r="C74" s="32"/>
       <c r="D74" s="33"/>
@@ -9564,8 +9577,8 @@
       <c r="AS74" s="32"/>
       <c r="AT74" s="33"/>
     </row>
-    <row r="75" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A75" s="204"/>
+    <row r="75" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A75" s="197"/>
       <c r="B75" s="42"/>
       <c r="C75" s="32"/>
       <c r="D75" s="33"/>
@@ -9628,8 +9641,8 @@
       <c r="AS75" s="32"/>
       <c r="AT75" s="33"/>
     </row>
-    <row r="76" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A76" s="204"/>
+    <row r="76" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A76" s="197"/>
       <c r="B76" s="42"/>
       <c r="C76" s="32"/>
       <c r="D76" s="33"/>
@@ -9687,8 +9700,8 @@
       <c r="AS76" s="32"/>
       <c r="AT76" s="33"/>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A77" s="203"/>
+    <row r="77" spans="1:46" ht="14" x14ac:dyDescent="0.15">
+      <c r="A77" s="196"/>
       <c r="B77" s="1"/>
       <c r="C77" s="2"/>
       <c r="D77" s="3"/>
@@ -9738,7 +9751,7 @@
       <c r="AS77" s="2"/>
       <c r="AT77" s="3"/>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A78" s="57" t="s">
         <v>32</v>
       </c>
@@ -9788,7 +9801,7 @@
       <c r="AS78" s="5"/>
       <c r="AT78" s="6"/>
     </row>
-    <row r="79" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A79" s="57" t="s">
         <v>33</v>
       </c>
@@ -9892,7 +9905,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A80" s="57" t="s">
         <v>34</v>
       </c>
@@ -10002,7 +10015,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="57" t="s">
         <v>35</v>
       </c>
@@ -10052,7 +10065,7 @@
       <c r="AS81" s="5"/>
       <c r="AT81" s="6"/>
     </row>
-    <row r="82" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="57" t="s">
         <v>36</v>
       </c>
@@ -10102,7 +10115,7 @@
       <c r="AS82" s="5"/>
       <c r="AT82" s="6"/>
     </row>
-    <row r="83" spans="1:46" ht="26" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A83" s="57" t="s">
         <v>37</v>
       </c>
@@ -10164,8 +10177,8 @@
       <c r="AS83" s="5"/>
       <c r="AT83" s="6"/>
     </row>
-    <row r="84" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A84" s="202" t="s">
+    <row r="84" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A84" s="195" t="s">
         <v>117</v>
       </c>
       <c r="B84" s="7"/>
@@ -10274,8 +10287,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A85" s="204"/>
+    <row r="85" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A85" s="197"/>
       <c r="B85" s="42"/>
       <c r="C85" s="32"/>
       <c r="D85" s="33"/>
@@ -10375,8 +10388,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A86" s="204"/>
+    <row r="86" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A86" s="197"/>
       <c r="B86" s="42"/>
       <c r="C86" s="32"/>
       <c r="D86" s="33"/>
@@ -10469,8 +10482,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A87" s="203"/>
+    <row r="87" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A87" s="196"/>
       <c r="B87" s="1"/>
       <c r="C87" s="2"/>
       <c r="D87" s="3"/>
@@ -10532,7 +10545,7 @@
       <c r="AS87" s="2"/>
       <c r="AT87" s="38"/>
     </row>
-    <row r="88" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="58" t="s">
         <v>38</v>
       </c>
@@ -10582,8 +10595,8 @@
       <c r="AS88" s="5"/>
       <c r="AT88" s="6"/>
     </row>
-    <row r="89" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A89" s="196" t="s">
+    <row r="89" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A89" s="188" t="s">
         <v>39</v>
       </c>
       <c r="B89" s="7"/>
@@ -10668,8 +10681,8 @@
       <c r="AS89" s="8"/>
       <c r="AT89" s="9"/>
     </row>
-    <row r="90" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A90" s="198"/>
+    <row r="90" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A90" s="190"/>
       <c r="B90" s="1"/>
       <c r="C90" s="2"/>
       <c r="D90" s="3"/>
@@ -10740,8 +10753,8 @@
       <c r="AS90" s="2"/>
       <c r="AT90" s="3"/>
     </row>
-    <row r="91" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A91" s="202" t="s">
+    <row r="91" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A91" s="195" t="s">
         <v>40</v>
       </c>
       <c r="B91" s="7"/>
@@ -10850,8 +10863,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A92" s="204"/>
+    <row r="92" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A92" s="197"/>
       <c r="B92" s="42"/>
       <c r="C92" s="32"/>
       <c r="D92" s="33"/>
@@ -10951,8 +10964,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A93" s="203"/>
+    <row r="93" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A93" s="196"/>
       <c r="B93" s="1"/>
       <c r="C93" s="2"/>
       <c r="D93" s="3"/>
@@ -11035,8 +11048,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="94" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A94" s="202" t="s">
+    <row r="94" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A94" s="195" t="s">
         <v>41</v>
       </c>
       <c r="B94" s="7"/>
@@ -11127,8 +11140,8 @@
       <c r="AS94" s="8"/>
       <c r="AT94" s="9"/>
     </row>
-    <row r="95" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A95" s="203"/>
+    <row r="95" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A95" s="196"/>
       <c r="B95" s="1"/>
       <c r="C95" s="2"/>
       <c r="D95" s="3"/>
@@ -11205,7 +11218,7 @@
       <c r="AS95" s="2"/>
       <c r="AT95" s="3"/>
     </row>
-    <row r="96" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A96" s="58" t="s">
         <v>42</v>
       </c>
@@ -11255,8 +11268,8 @@
       <c r="AS96" s="5"/>
       <c r="AT96" s="6"/>
     </row>
-    <row r="97" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A97" s="196" t="s">
+    <row r="97" spans="1:46" ht="56" x14ac:dyDescent="0.15">
+      <c r="A97" s="188" t="s">
         <v>43</v>
       </c>
       <c r="B97" s="7"/>
@@ -11365,8 +11378,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:46" ht="52" x14ac:dyDescent="0.15">
-      <c r="A98" s="197"/>
+    <row r="98" spans="1:46" ht="56" x14ac:dyDescent="0.15">
+      <c r="A98" s="189"/>
       <c r="B98" s="42"/>
       <c r="C98" s="32"/>
       <c r="D98" s="33"/>
@@ -11452,8 +11465,8 @@
       <c r="AS98" s="32"/>
       <c r="AT98" s="33"/>
     </row>
-    <row r="99" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A99" s="197"/>
+    <row r="99" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A99" s="189"/>
       <c r="B99" s="42"/>
       <c r="C99" s="32"/>
       <c r="D99" s="33"/>
@@ -11532,8 +11545,8 @@
       <c r="AS99" s="32"/>
       <c r="AT99" s="33"/>
     </row>
-    <row r="100" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A100" s="197"/>
+    <row r="100" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A100" s="189"/>
       <c r="B100" s="42"/>
       <c r="C100" s="32"/>
       <c r="D100" s="33"/>
@@ -11612,8 +11625,8 @@
       <c r="AS100" s="32"/>
       <c r="AT100" s="33"/>
     </row>
-    <row r="101" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A101" s="197"/>
+    <row r="101" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A101" s="189"/>
       <c r="B101" s="42"/>
       <c r="C101" s="32"/>
       <c r="D101" s="33"/>
@@ -11685,8 +11698,8 @@
       <c r="AS101" s="32"/>
       <c r="AT101" s="33"/>
     </row>
-    <row r="102" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A102" s="197"/>
+    <row r="102" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A102" s="189"/>
       <c r="B102" s="42"/>
       <c r="C102" s="32"/>
       <c r="D102" s="33"/>
@@ -11758,8 +11771,8 @@
       <c r="AS102" s="32"/>
       <c r="AT102" s="33"/>
     </row>
-    <row r="103" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A103" s="197"/>
+    <row r="103" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A103" s="189"/>
       <c r="B103" s="42"/>
       <c r="C103" s="32"/>
       <c r="D103" s="33"/>
@@ -11831,8 +11844,8 @@
       <c r="AS103" s="32"/>
       <c r="AT103" s="33"/>
     </row>
-    <row r="104" spans="1:46" ht="39" x14ac:dyDescent="0.15">
-      <c r="A104" s="197"/>
+    <row r="104" spans="1:46" ht="42" x14ac:dyDescent="0.15">
+      <c r="A104" s="189"/>
       <c r="B104" s="42"/>
       <c r="C104" s="32"/>
       <c r="D104" s="33"/>
@@ -11904,8 +11917,8 @@
       <c r="AS104" s="32"/>
       <c r="AT104" s="33"/>
     </row>
-    <row r="105" spans="1:46" ht="26" x14ac:dyDescent="0.15">
-      <c r="A105" s="198"/>
+    <row r="105" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A105" s="190"/>
       <c r="B105" s="1"/>
       <c r="C105" s="2"/>
       <c r="D105" s="3"/>
@@ -11973,7 +11986,7 @@
       <c r="AS105" s="2"/>
       <c r="AT105" s="3"/>
     </row>
-    <row r="106" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A106" s="53" t="s">
         <v>44</v>
       </c>
@@ -12023,7 +12036,7 @@
       <c r="AS106" s="8"/>
       <c r="AT106" s="9"/>
     </row>
-    <row r="107" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="54" t="s">
         <v>45</v>
       </c>
@@ -12061,7 +12074,7 @@
       <c r="AS107" s="32"/>
       <c r="AT107" s="33"/>
     </row>
-    <row r="108" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="54" t="s">
         <v>46</v>
       </c>
@@ -12099,7 +12112,7 @@
       <c r="AS108" s="32"/>
       <c r="AT108" s="33"/>
     </row>
-    <row r="109" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A109" s="55" t="s">
         <v>47</v>
       </c>
@@ -12171,69 +12184,69 @@
       <c r="Q110" s="165"/>
     </row>
     <row r="111" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="190" t="s">
+      <c r="A111" s="203" t="s">
         <v>393</v>
       </c>
-      <c r="B111" s="190"/>
-      <c r="C111" s="190"/>
-      <c r="D111" s="190"/>
-      <c r="E111" s="190"/>
-      <c r="F111" s="190"/>
-      <c r="G111" s="190"/>
-      <c r="H111" s="190"/>
-      <c r="I111" s="190"/>
-      <c r="J111" s="190"/>
-      <c r="K111" s="190"/>
-      <c r="L111" s="190"/>
-      <c r="M111" s="190"/>
-      <c r="N111" s="190"/>
-      <c r="O111" s="190"/>
-      <c r="P111" s="190"/>
-      <c r="Q111" s="190"/>
-      <c r="R111" s="190"/>
-      <c r="S111" s="190"/>
-      <c r="T111" s="190"/>
-      <c r="U111" s="190"/>
-      <c r="V111" s="190"/>
-      <c r="W111" s="190"/>
-      <c r="X111" s="190"/>
-      <c r="Y111" s="190"/>
-      <c r="Z111" s="190"/>
-      <c r="AA111" s="190"/>
-      <c r="AB111" s="190"/>
-      <c r="AC111" s="190"/>
-      <c r="AD111" s="190"/>
-      <c r="AE111" s="190"/>
-      <c r="AF111" s="190"/>
-      <c r="AG111" s="190"/>
-      <c r="AH111" s="190"/>
-      <c r="AI111" s="190"/>
-      <c r="AJ111" s="190"/>
-      <c r="AK111" s="190"/>
-      <c r="AL111" s="190"/>
-      <c r="AM111" s="190"/>
-      <c r="AN111" s="190"/>
-      <c r="AO111" s="190"/>
-      <c r="AP111" s="190"/>
-      <c r="AQ111" s="190"/>
-      <c r="AR111" s="190"/>
-      <c r="AS111" s="190"/>
-      <c r="AT111" s="190"/>
+      <c r="B111" s="203"/>
+      <c r="C111" s="203"/>
+      <c r="D111" s="203"/>
+      <c r="E111" s="203"/>
+      <c r="F111" s="203"/>
+      <c r="G111" s="203"/>
+      <c r="H111" s="203"/>
+      <c r="I111" s="203"/>
+      <c r="J111" s="203"/>
+      <c r="K111" s="203"/>
+      <c r="L111" s="203"/>
+      <c r="M111" s="203"/>
+      <c r="N111" s="203"/>
+      <c r="O111" s="203"/>
+      <c r="P111" s="203"/>
+      <c r="Q111" s="203"/>
+      <c r="R111" s="203"/>
+      <c r="S111" s="203"/>
+      <c r="T111" s="203"/>
+      <c r="U111" s="203"/>
+      <c r="V111" s="203"/>
+      <c r="W111" s="203"/>
+      <c r="X111" s="203"/>
+      <c r="Y111" s="203"/>
+      <c r="Z111" s="203"/>
+      <c r="AA111" s="203"/>
+      <c r="AB111" s="203"/>
+      <c r="AC111" s="203"/>
+      <c r="AD111" s="203"/>
+      <c r="AE111" s="203"/>
+      <c r="AF111" s="203"/>
+      <c r="AG111" s="203"/>
+      <c r="AH111" s="203"/>
+      <c r="AI111" s="203"/>
+      <c r="AJ111" s="203"/>
+      <c r="AK111" s="203"/>
+      <c r="AL111" s="203"/>
+      <c r="AM111" s="203"/>
+      <c r="AN111" s="203"/>
+      <c r="AO111" s="203"/>
+      <c r="AP111" s="203"/>
+      <c r="AQ111" s="203"/>
+      <c r="AR111" s="203"/>
+      <c r="AS111" s="203"/>
+      <c r="AT111" s="203"/>
     </row>
     <row r="112" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A112" s="188" t="s">
+      <c r="A112" s="201" t="s">
         <v>375</v>
       </c>
-      <c r="B112" s="188"/>
-      <c r="C112" s="188"/>
-      <c r="D112" s="188"/>
-      <c r="E112" s="188"/>
-      <c r="F112" s="188"/>
-      <c r="G112" s="188"/>
-      <c r="H112" s="188"/>
-      <c r="I112" s="188"/>
-      <c r="J112" s="188"/>
-      <c r="K112" s="188"/>
+      <c r="B112" s="201"/>
+      <c r="C112" s="201"/>
+      <c r="D112" s="201"/>
+      <c r="E112" s="201"/>
+      <c r="F112" s="201"/>
+      <c r="G112" s="201"/>
+      <c r="H112" s="201"/>
+      <c r="I112" s="201"/>
+      <c r="J112" s="201"/>
+      <c r="K112" s="201"/>
       <c r="L112" s="61"/>
       <c r="M112" s="61"/>
       <c r="N112" s="61"/>
@@ -12268,154 +12281,154 @@
       <c r="AQ112" s="61"/>
     </row>
     <row r="113" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A113" s="189" t="s">
+      <c r="A113" s="202" t="s">
         <v>376</v>
       </c>
-      <c r="B113" s="189"/>
-      <c r="C113" s="189"/>
-      <c r="D113" s="189"/>
-      <c r="E113" s="189"/>
-      <c r="F113" s="189"/>
-      <c r="G113" s="189"/>
-      <c r="H113" s="189"/>
-      <c r="I113" s="189"/>
-      <c r="J113" s="189"/>
-      <c r="K113" s="189"/>
-      <c r="L113" s="189"/>
-      <c r="M113" s="189"/>
-      <c r="N113" s="189"/>
-      <c r="O113" s="189"/>
-      <c r="P113" s="189"/>
-      <c r="Q113" s="189"/>
-      <c r="R113" s="189"/>
-      <c r="S113" s="189"/>
-      <c r="T113" s="189"/>
-      <c r="U113" s="189"/>
-      <c r="V113" s="189"/>
-      <c r="W113" s="189"/>
-      <c r="X113" s="189"/>
-      <c r="Y113" s="189"/>
-      <c r="Z113" s="189"/>
-      <c r="AA113" s="189"/>
-      <c r="AB113" s="189"/>
-      <c r="AC113" s="189"/>
-      <c r="AD113" s="189"/>
-      <c r="AE113" s="189"/>
-      <c r="AF113" s="189"/>
-      <c r="AG113" s="189"/>
-      <c r="AH113" s="189"/>
-      <c r="AI113" s="189"/>
-      <c r="AJ113" s="189"/>
-      <c r="AK113" s="189"/>
-      <c r="AL113" s="189"/>
-      <c r="AM113" s="189"/>
-      <c r="AN113" s="189"/>
-      <c r="AO113" s="189"/>
-      <c r="AP113" s="189"/>
-      <c r="AQ113" s="189"/>
-      <c r="AR113" s="189"/>
-      <c r="AS113" s="189"/>
-      <c r="AT113" s="189"/>
+      <c r="B113" s="202"/>
+      <c r="C113" s="202"/>
+      <c r="D113" s="202"/>
+      <c r="E113" s="202"/>
+      <c r="F113" s="202"/>
+      <c r="G113" s="202"/>
+      <c r="H113" s="202"/>
+      <c r="I113" s="202"/>
+      <c r="J113" s="202"/>
+      <c r="K113" s="202"/>
+      <c r="L113" s="202"/>
+      <c r="M113" s="202"/>
+      <c r="N113" s="202"/>
+      <c r="O113" s="202"/>
+      <c r="P113" s="202"/>
+      <c r="Q113" s="202"/>
+      <c r="R113" s="202"/>
+      <c r="S113" s="202"/>
+      <c r="T113" s="202"/>
+      <c r="U113" s="202"/>
+      <c r="V113" s="202"/>
+      <c r="W113" s="202"/>
+      <c r="X113" s="202"/>
+      <c r="Y113" s="202"/>
+      <c r="Z113" s="202"/>
+      <c r="AA113" s="202"/>
+      <c r="AB113" s="202"/>
+      <c r="AC113" s="202"/>
+      <c r="AD113" s="202"/>
+      <c r="AE113" s="202"/>
+      <c r="AF113" s="202"/>
+      <c r="AG113" s="202"/>
+      <c r="AH113" s="202"/>
+      <c r="AI113" s="202"/>
+      <c r="AJ113" s="202"/>
+      <c r="AK113" s="202"/>
+      <c r="AL113" s="202"/>
+      <c r="AM113" s="202"/>
+      <c r="AN113" s="202"/>
+      <c r="AO113" s="202"/>
+      <c r="AP113" s="202"/>
+      <c r="AQ113" s="202"/>
+      <c r="AR113" s="202"/>
+      <c r="AS113" s="202"/>
+      <c r="AT113" s="202"/>
     </row>
     <row r="114" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A114" s="192" t="s">
+      <c r="A114" s="205" t="s">
         <v>377</v>
       </c>
-      <c r="B114" s="192"/>
-      <c r="C114" s="192"/>
-      <c r="D114" s="192"/>
-      <c r="E114" s="192"/>
-      <c r="F114" s="192"/>
-      <c r="G114" s="192"/>
-      <c r="H114" s="192"/>
-      <c r="I114" s="192"/>
-      <c r="J114" s="192"/>
-      <c r="K114" s="192"/>
-      <c r="L114" s="192"/>
-      <c r="M114" s="192"/>
-      <c r="N114" s="192"/>
-      <c r="O114" s="192"/>
-      <c r="P114" s="192"/>
-      <c r="Q114" s="192"/>
-      <c r="R114" s="192"/>
-      <c r="S114" s="192"/>
-      <c r="T114" s="192"/>
-      <c r="U114" s="192"/>
-      <c r="V114" s="192"/>
-      <c r="W114" s="192"/>
-      <c r="X114" s="192"/>
-      <c r="Y114" s="192"/>
-      <c r="Z114" s="192"/>
-      <c r="AA114" s="192"/>
-      <c r="AB114" s="192"/>
-      <c r="AC114" s="192"/>
-      <c r="AD114" s="192"/>
-      <c r="AE114" s="192"/>
-      <c r="AF114" s="192"/>
-      <c r="AG114" s="192"/>
-      <c r="AH114" s="192"/>
-      <c r="AI114" s="192"/>
-      <c r="AJ114" s="192"/>
-      <c r="AK114" s="192"/>
-      <c r="AL114" s="192"/>
-      <c r="AM114" s="192"/>
-      <c r="AN114" s="192"/>
-      <c r="AO114" s="192"/>
-      <c r="AP114" s="192"/>
-      <c r="AQ114" s="192"/>
-      <c r="AR114" s="192"/>
-      <c r="AS114" s="192"/>
-      <c r="AT114" s="192"/>
+      <c r="B114" s="205"/>
+      <c r="C114" s="205"/>
+      <c r="D114" s="205"/>
+      <c r="E114" s="205"/>
+      <c r="F114" s="205"/>
+      <c r="G114" s="205"/>
+      <c r="H114" s="205"/>
+      <c r="I114" s="205"/>
+      <c r="J114" s="205"/>
+      <c r="K114" s="205"/>
+      <c r="L114" s="205"/>
+      <c r="M114" s="205"/>
+      <c r="N114" s="205"/>
+      <c r="O114" s="205"/>
+      <c r="P114" s="205"/>
+      <c r="Q114" s="205"/>
+      <c r="R114" s="205"/>
+      <c r="S114" s="205"/>
+      <c r="T114" s="205"/>
+      <c r="U114" s="205"/>
+      <c r="V114" s="205"/>
+      <c r="W114" s="205"/>
+      <c r="X114" s="205"/>
+      <c r="Y114" s="205"/>
+      <c r="Z114" s="205"/>
+      <c r="AA114" s="205"/>
+      <c r="AB114" s="205"/>
+      <c r="AC114" s="205"/>
+      <c r="AD114" s="205"/>
+      <c r="AE114" s="205"/>
+      <c r="AF114" s="205"/>
+      <c r="AG114" s="205"/>
+      <c r="AH114" s="205"/>
+      <c r="AI114" s="205"/>
+      <c r="AJ114" s="205"/>
+      <c r="AK114" s="205"/>
+      <c r="AL114" s="205"/>
+      <c r="AM114" s="205"/>
+      <c r="AN114" s="205"/>
+      <c r="AO114" s="205"/>
+      <c r="AP114" s="205"/>
+      <c r="AQ114" s="205"/>
+      <c r="AR114" s="205"/>
+      <c r="AS114" s="205"/>
+      <c r="AT114" s="205"/>
     </row>
     <row r="115" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A115" s="191" t="s">
+      <c r="A115" s="204" t="s">
         <v>336</v>
       </c>
-      <c r="B115" s="191"/>
-      <c r="C115" s="191"/>
-      <c r="D115" s="191"/>
-      <c r="E115" s="191"/>
-      <c r="F115" s="191"/>
-      <c r="G115" s="191"/>
-      <c r="H115" s="191"/>
-      <c r="I115" s="191"/>
-      <c r="J115" s="191"/>
-      <c r="K115" s="191"/>
-      <c r="L115" s="191"/>
-      <c r="M115" s="191"/>
-      <c r="N115" s="191"/>
-      <c r="O115" s="191"/>
-      <c r="P115" s="191"/>
-      <c r="Q115" s="191"/>
-      <c r="R115" s="191"/>
-      <c r="S115" s="191"/>
-      <c r="T115" s="191"/>
-      <c r="U115" s="191"/>
-      <c r="V115" s="191"/>
-      <c r="W115" s="191"/>
-      <c r="X115" s="191"/>
-      <c r="Y115" s="191"/>
-      <c r="Z115" s="191"/>
-      <c r="AA115" s="191"/>
-      <c r="AB115" s="191"/>
-      <c r="AC115" s="191"/>
-      <c r="AD115" s="191"/>
-      <c r="AE115" s="191"/>
-      <c r="AF115" s="191"/>
-      <c r="AG115" s="191"/>
-      <c r="AH115" s="191"/>
-      <c r="AI115" s="191"/>
-      <c r="AJ115" s="191"/>
-      <c r="AK115" s="191"/>
-      <c r="AL115" s="191"/>
-      <c r="AM115" s="191"/>
-      <c r="AN115" s="191"/>
-      <c r="AO115" s="191"/>
-      <c r="AP115" s="191"/>
-      <c r="AQ115" s="191"/>
-      <c r="AR115" s="191"/>
-      <c r="AS115" s="191"/>
-      <c r="AT115" s="191"/>
+      <c r="B115" s="204"/>
+      <c r="C115" s="204"/>
+      <c r="D115" s="204"/>
+      <c r="E115" s="204"/>
+      <c r="F115" s="204"/>
+      <c r="G115" s="204"/>
+      <c r="H115" s="204"/>
+      <c r="I115" s="204"/>
+      <c r="J115" s="204"/>
+      <c r="K115" s="204"/>
+      <c r="L115" s="204"/>
+      <c r="M115" s="204"/>
+      <c r="N115" s="204"/>
+      <c r="O115" s="204"/>
+      <c r="P115" s="204"/>
+      <c r="Q115" s="204"/>
+      <c r="R115" s="204"/>
+      <c r="S115" s="204"/>
+      <c r="T115" s="204"/>
+      <c r="U115" s="204"/>
+      <c r="V115" s="204"/>
+      <c r="W115" s="204"/>
+      <c r="X115" s="204"/>
+      <c r="Y115" s="204"/>
+      <c r="Z115" s="204"/>
+      <c r="AA115" s="204"/>
+      <c r="AB115" s="204"/>
+      <c r="AC115" s="204"/>
+      <c r="AD115" s="204"/>
+      <c r="AE115" s="204"/>
+      <c r="AF115" s="204"/>
+      <c r="AG115" s="204"/>
+      <c r="AH115" s="204"/>
+      <c r="AI115" s="204"/>
+      <c r="AJ115" s="204"/>
+      <c r="AK115" s="204"/>
+      <c r="AL115" s="204"/>
+      <c r="AM115" s="204"/>
+      <c r="AN115" s="204"/>
+      <c r="AO115" s="204"/>
+      <c r="AP115" s="204"/>
+      <c r="AQ115" s="204"/>
+      <c r="AR115" s="204"/>
+      <c r="AS115" s="204"/>
+      <c r="AT115" s="204"/>
     </row>
     <row r="116" spans="1:46" ht="15" x14ac:dyDescent="0.2">
       <c r="A116"/>
@@ -12557,6 +12570,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A112:K112"/>
+    <mergeCell ref="A113:AT113"/>
+    <mergeCell ref="A111:AT111"/>
+    <mergeCell ref="A115:AT115"/>
+    <mergeCell ref="A114:AT114"/>
+    <mergeCell ref="AR2:AT2"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A69:A77"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="A21:A24"/>
     <mergeCell ref="A97:A105"/>
     <mergeCell ref="A1:AQ1"/>
     <mergeCell ref="A25:A26"/>
@@ -12573,28 +12608,6 @@
     <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="AL2:AN2"/>
     <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A69:A77"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A7:A16"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="AR2:AT2"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="A112:K112"/>
-    <mergeCell ref="A113:AT113"/>
-    <mergeCell ref="A111:AT111"/>
-    <mergeCell ref="A115:AT115"/>
-    <mergeCell ref="A114:AT114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="19" fitToWidth="4" fitToHeight="3" orientation="landscape"/>
@@ -12602,8 +12615,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:U59"/>
@@ -15660,8 +15673,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:Q40"/>
@@ -15688,24 +15701,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="70" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="263" t="s">
+      <c r="A1" s="236" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="263"/>
-      <c r="J1" s="263"/>
-      <c r="K1" s="263"/>
-      <c r="L1" s="263"/>
-      <c r="M1" s="263"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
     </row>
     <row r="2" spans="1:13" s="70" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="248"/>
+      <c r="A2" s="265"/>
       <c r="B2" s="223">
         <v>2010</v>
       </c>
@@ -15726,7 +15739,7 @@
       <c r="M2" s="223"/>
     </row>
     <row r="3" spans="1:13" s="70" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="248"/>
+      <c r="A3" s="265"/>
       <c r="B3" s="109" t="s">
         <v>240</v>
       </c>
@@ -15764,377 +15777,377 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A4" s="233" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="236"/>
-      <c r="C4" s="239"/>
-      <c r="D4" s="236"/>
-      <c r="E4" s="236"/>
-      <c r="F4" s="242" t="s">
+    <row r="4" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A4" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="243"/>
+      <c r="C4" s="262"/>
+      <c r="D4" s="243"/>
+      <c r="E4" s="243"/>
+      <c r="F4" s="239" t="s">
         <v>244</v>
       </c>
-      <c r="G4" s="245">
+      <c r="G4" s="241">
         <v>40695</v>
       </c>
-      <c r="H4" s="245">
+      <c r="H4" s="241">
         <v>40787</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="J4" s="242" t="s">
+      <c r="J4" s="239" t="s">
         <v>245</v>
       </c>
-      <c r="K4" s="245">
+      <c r="K4" s="241">
         <v>41030</v>
       </c>
-      <c r="L4" s="245">
+      <c r="L4" s="241">
         <v>41030</v>
       </c>
       <c r="M4" s="176" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="39" x14ac:dyDescent="0.15">
-      <c r="A5" s="234"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="240"/>
-      <c r="D5" s="237"/>
-      <c r="E5" s="237"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="246"/>
-      <c r="H5" s="246"/>
+    <row r="5" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A5" s="252"/>
+      <c r="B5" s="246"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="246"/>
+      <c r="E5" s="246"/>
+      <c r="F5" s="247"/>
+      <c r="G5" s="242"/>
+      <c r="H5" s="242"/>
       <c r="I5" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="J5" s="243"/>
-      <c r="K5" s="246"/>
-      <c r="L5" s="246"/>
+      <c r="J5" s="247"/>
+      <c r="K5" s="242"/>
+      <c r="L5" s="242"/>
       <c r="M5" s="12" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A6" s="234"/>
-      <c r="B6" s="237"/>
-      <c r="C6" s="240"/>
-      <c r="D6" s="237"/>
-      <c r="E6" s="237"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="246"/>
-      <c r="H6" s="246"/>
+    <row r="6" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A6" s="252"/>
+      <c r="B6" s="246"/>
+      <c r="C6" s="263"/>
+      <c r="D6" s="246"/>
+      <c r="E6" s="246"/>
+      <c r="F6" s="247"/>
+      <c r="G6" s="242"/>
+      <c r="H6" s="242"/>
       <c r="I6" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="J6" s="243"/>
-      <c r="K6" s="246"/>
-      <c r="L6" s="246"/>
+      <c r="J6" s="247"/>
+      <c r="K6" s="242"/>
+      <c r="L6" s="242"/>
       <c r="M6" s="175" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A7" s="234"/>
-      <c r="B7" s="237"/>
-      <c r="C7" s="240"/>
-      <c r="D7" s="237"/>
-      <c r="E7" s="237"/>
-      <c r="F7" s="243"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
+    <row r="7" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A7" s="252"/>
+      <c r="B7" s="246"/>
+      <c r="C7" s="263"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="247"/>
+      <c r="G7" s="242"/>
+      <c r="H7" s="242"/>
       <c r="I7" s="175" t="s">
         <v>414</v>
       </c>
-      <c r="J7" s="243"/>
-      <c r="K7" s="246"/>
-      <c r="L7" s="246"/>
+      <c r="J7" s="247"/>
+      <c r="K7" s="242"/>
+      <c r="L7" s="242"/>
       <c r="M7" s="175" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="234"/>
-      <c r="B8" s="237"/>
-      <c r="C8" s="240"/>
-      <c r="D8" s="237"/>
-      <c r="E8" s="237"/>
-      <c r="F8" s="243"/>
-      <c r="G8" s="246"/>
-      <c r="H8" s="246"/>
+      <c r="A8" s="252"/>
+      <c r="B8" s="246"/>
+      <c r="C8" s="263"/>
+      <c r="D8" s="246"/>
+      <c r="E8" s="246"/>
+      <c r="F8" s="247"/>
+      <c r="G8" s="242"/>
+      <c r="H8" s="242"/>
       <c r="I8" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="J8" s="243"/>
-      <c r="K8" s="246"/>
-      <c r="L8" s="246"/>
+      <c r="J8" s="247"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="242"/>
       <c r="M8" s="13" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A9" s="235"/>
-      <c r="B9" s="238"/>
-      <c r="C9" s="241"/>
-      <c r="D9" s="238"/>
-      <c r="E9" s="238"/>
-      <c r="F9" s="244"/>
-      <c r="G9" s="247"/>
-      <c r="H9" s="247"/>
+    <row r="9" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A9" s="253"/>
+      <c r="B9" s="244"/>
+      <c r="C9" s="264"/>
+      <c r="D9" s="244"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="240"/>
+      <c r="G9" s="245"/>
+      <c r="H9" s="245"/>
       <c r="I9" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="J9" s="244"/>
-      <c r="K9" s="247"/>
-      <c r="L9" s="247"/>
+      <c r="J9" s="240"/>
+      <c r="K9" s="245"/>
+      <c r="L9" s="245"/>
       <c r="M9" s="14" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="78" x14ac:dyDescent="0.15">
-      <c r="A10" s="233" t="s">
+    <row r="10" spans="1:13" ht="98" x14ac:dyDescent="0.15">
+      <c r="A10" s="251" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="254" t="s">
+      <c r="B10" s="248" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="257">
+      <c r="C10" s="259">
         <v>40360</v>
       </c>
-      <c r="D10" s="257">
+      <c r="D10" s="259">
         <v>40360</v>
       </c>
       <c r="E10" s="172" t="s">
         <v>407</v>
       </c>
-      <c r="F10" s="249"/>
-      <c r="G10" s="249"/>
-      <c r="H10" s="249"/>
-      <c r="I10" s="249"/>
-      <c r="J10" s="249"/>
-      <c r="K10" s="249"/>
-      <c r="L10" s="249"/>
+      <c r="F10" s="254"/>
+      <c r="G10" s="254"/>
+      <c r="H10" s="254"/>
+      <c r="I10" s="254"/>
+      <c r="J10" s="254"/>
+      <c r="K10" s="254"/>
+      <c r="L10" s="254"/>
       <c r="M10" s="157"/>
     </row>
-    <row r="11" spans="1:13" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="234"/>
-      <c r="B11" s="255"/>
-      <c r="C11" s="258"/>
-      <c r="D11" s="258"/>
+    <row r="11" spans="1:13" ht="28" x14ac:dyDescent="0.15">
+      <c r="A11" s="252"/>
+      <c r="B11" s="249"/>
+      <c r="C11" s="260"/>
+      <c r="D11" s="260"/>
       <c r="E11" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="F11" s="250"/>
-      <c r="G11" s="250"/>
-      <c r="H11" s="250"/>
-      <c r="I11" s="250"/>
-      <c r="J11" s="250"/>
-      <c r="K11" s="250"/>
-      <c r="L11" s="250"/>
+      <c r="F11" s="255"/>
+      <c r="G11" s="255"/>
+      <c r="H11" s="255"/>
+      <c r="I11" s="255"/>
+      <c r="J11" s="255"/>
+      <c r="K11" s="255"/>
+      <c r="L11" s="255"/>
       <c r="M11" s="158"/>
     </row>
-    <row r="12" spans="1:13" ht="39" x14ac:dyDescent="0.15">
-      <c r="A12" s="234"/>
-      <c r="B12" s="255"/>
-      <c r="C12" s="258"/>
-      <c r="D12" s="258"/>
+    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A12" s="252"/>
+      <c r="B12" s="249"/>
+      <c r="C12" s="260"/>
+      <c r="D12" s="260"/>
       <c r="E12" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="F12" s="250"/>
-      <c r="G12" s="250"/>
-      <c r="H12" s="250"/>
-      <c r="I12" s="250"/>
-      <c r="J12" s="250"/>
-      <c r="K12" s="250"/>
-      <c r="L12" s="250"/>
+      <c r="F12" s="255"/>
+      <c r="G12" s="255"/>
+      <c r="H12" s="255"/>
+      <c r="I12" s="255"/>
+      <c r="J12" s="255"/>
+      <c r="K12" s="255"/>
+      <c r="L12" s="255"/>
       <c r="M12" s="159"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="235"/>
-      <c r="B13" s="256"/>
-      <c r="C13" s="259"/>
-      <c r="D13" s="259"/>
+    <row r="13" spans="1:13" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="253"/>
+      <c r="B13" s="250"/>
+      <c r="C13" s="261"/>
+      <c r="D13" s="261"/>
       <c r="E13" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="F13" s="251"/>
-      <c r="G13" s="251"/>
-      <c r="H13" s="251"/>
-      <c r="I13" s="251"/>
-      <c r="J13" s="251"/>
-      <c r="K13" s="251"/>
-      <c r="L13" s="251"/>
+      <c r="F13" s="256"/>
+      <c r="G13" s="256"/>
+      <c r="H13" s="256"/>
+      <c r="I13" s="256"/>
+      <c r="J13" s="256"/>
+      <c r="K13" s="256"/>
+      <c r="L13" s="256"/>
       <c r="M13" s="160"/>
     </row>
-    <row r="14" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A14" s="252" t="s">
+    <row r="14" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A14" s="257" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="236"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="236"/>
-      <c r="F14" s="242" t="s">
+      <c r="B14" s="243"/>
+      <c r="C14" s="243"/>
+      <c r="D14" s="243"/>
+      <c r="E14" s="243"/>
+      <c r="F14" s="239" t="s">
         <v>246</v>
       </c>
-      <c r="G14" s="245">
+      <c r="G14" s="241">
         <v>40664</v>
       </c>
-      <c r="H14" s="245">
+      <c r="H14" s="241">
         <v>40725</v>
       </c>
       <c r="I14" s="172" t="s">
         <v>412</v>
       </c>
-      <c r="J14" s="236"/>
-      <c r="K14" s="236"/>
-      <c r="L14" s="236"/>
+      <c r="J14" s="243"/>
+      <c r="K14" s="243"/>
+      <c r="L14" s="243"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13" ht="26" x14ac:dyDescent="0.15">
-      <c r="A15" s="253"/>
-      <c r="B15" s="237"/>
-      <c r="C15" s="237"/>
-      <c r="D15" s="237"/>
-      <c r="E15" s="237"/>
-      <c r="F15" s="243"/>
-      <c r="G15" s="246"/>
-      <c r="H15" s="246"/>
+    <row r="15" spans="1:13" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" s="258"/>
+      <c r="B15" s="246"/>
+      <c r="C15" s="246"/>
+      <c r="D15" s="246"/>
+      <c r="E15" s="246"/>
+      <c r="F15" s="247"/>
+      <c r="G15" s="242"/>
+      <c r="H15" s="242"/>
       <c r="I15" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="J15" s="237"/>
-      <c r="K15" s="237"/>
-      <c r="L15" s="237"/>
+      <c r="J15" s="246"/>
+      <c r="K15" s="246"/>
+      <c r="L15" s="246"/>
       <c r="M15" s="16"/>
     </row>
-    <row r="16" spans="1:13" ht="26" x14ac:dyDescent="0.15">
-      <c r="A16" s="253"/>
-      <c r="B16" s="237"/>
-      <c r="C16" s="237"/>
-      <c r="D16" s="237"/>
-      <c r="E16" s="237"/>
-      <c r="F16" s="243"/>
-      <c r="G16" s="246"/>
-      <c r="H16" s="246"/>
+    <row r="16" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A16" s="258"/>
+      <c r="B16" s="246"/>
+      <c r="C16" s="246"/>
+      <c r="D16" s="246"/>
+      <c r="E16" s="246"/>
+      <c r="F16" s="247"/>
+      <c r="G16" s="242"/>
+      <c r="H16" s="242"/>
       <c r="I16" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="J16" s="237"/>
-      <c r="K16" s="237"/>
-      <c r="L16" s="237"/>
+      <c r="J16" s="246"/>
+      <c r="K16" s="246"/>
+      <c r="L16" s="246"/>
       <c r="M16" s="16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A17" s="253"/>
-      <c r="B17" s="238"/>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
-      <c r="E17" s="238"/>
-      <c r="F17" s="244"/>
-      <c r="G17" s="247"/>
-      <c r="H17" s="247"/>
+    <row r="17" spans="1:13" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="258"/>
+      <c r="B17" s="244"/>
+      <c r="C17" s="244"/>
+      <c r="D17" s="244"/>
+      <c r="E17" s="244"/>
+      <c r="F17" s="240"/>
+      <c r="G17" s="245"/>
+      <c r="H17" s="245"/>
       <c r="I17" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="J17" s="238"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="238"/>
+      <c r="J17" s="244"/>
+      <c r="K17" s="244"/>
+      <c r="L17" s="244"/>
       <c r="M17" s="17"/>
     </row>
-    <row r="18" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A18" s="233" t="s">
+    <row r="18" spans="1:13" ht="70" x14ac:dyDescent="0.15">
+      <c r="A18" s="251" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="236"/>
-      <c r="C18" s="236"/>
-      <c r="D18" s="236"/>
-      <c r="E18" s="236"/>
-      <c r="F18" s="242" t="s">
+      <c r="B18" s="243"/>
+      <c r="C18" s="243"/>
+      <c r="D18" s="243"/>
+      <c r="E18" s="243"/>
+      <c r="F18" s="239" t="s">
         <v>247</v>
       </c>
-      <c r="G18" s="245">
+      <c r="G18" s="241">
         <v>40664</v>
       </c>
-      <c r="H18" s="245">
+      <c r="H18" s="241">
         <v>40725</v>
       </c>
       <c r="I18" s="172" t="s">
         <v>413</v>
       </c>
-      <c r="J18" s="236"/>
-      <c r="K18" s="236"/>
-      <c r="L18" s="236"/>
+      <c r="J18" s="243"/>
+      <c r="K18" s="243"/>
+      <c r="L18" s="243"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" ht="26" x14ac:dyDescent="0.15">
-      <c r="A19" s="234"/>
-      <c r="B19" s="237"/>
-      <c r="C19" s="237"/>
-      <c r="D19" s="237"/>
-      <c r="E19" s="237"/>
-      <c r="F19" s="243"/>
-      <c r="G19" s="243"/>
-      <c r="H19" s="243"/>
+    <row r="19" spans="1:13" ht="28" x14ac:dyDescent="0.15">
+      <c r="A19" s="252"/>
+      <c r="B19" s="246"/>
+      <c r="C19" s="246"/>
+      <c r="D19" s="246"/>
+      <c r="E19" s="246"/>
+      <c r="F19" s="247"/>
+      <c r="G19" s="247"/>
+      <c r="H19" s="247"/>
       <c r="I19" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="J19" s="237"/>
-      <c r="K19" s="237"/>
-      <c r="L19" s="237"/>
+      <c r="J19" s="246"/>
+      <c r="K19" s="246"/>
+      <c r="L19" s="246"/>
       <c r="M19" s="16"/>
     </row>
-    <row r="20" spans="1:13" ht="26" x14ac:dyDescent="0.15">
-      <c r="A20" s="234"/>
-      <c r="B20" s="237"/>
-      <c r="C20" s="237"/>
-      <c r="D20" s="237"/>
-      <c r="E20" s="237"/>
-      <c r="F20" s="243"/>
-      <c r="G20" s="243"/>
-      <c r="H20" s="243"/>
+    <row r="20" spans="1:13" ht="28" x14ac:dyDescent="0.15">
+      <c r="A20" s="252"/>
+      <c r="B20" s="246"/>
+      <c r="C20" s="246"/>
+      <c r="D20" s="246"/>
+      <c r="E20" s="246"/>
+      <c r="F20" s="247"/>
+      <c r="G20" s="247"/>
+      <c r="H20" s="247"/>
       <c r="I20" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="J20" s="237"/>
-      <c r="K20" s="237"/>
-      <c r="L20" s="237"/>
+      <c r="J20" s="246"/>
+      <c r="K20" s="246"/>
+      <c r="L20" s="246"/>
       <c r="M20" s="16"/>
     </row>
-    <row r="21" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A21" s="235"/>
-      <c r="B21" s="238"/>
-      <c r="C21" s="238"/>
-      <c r="D21" s="238"/>
-      <c r="E21" s="238"/>
-      <c r="F21" s="244"/>
-      <c r="G21" s="244"/>
-      <c r="H21" s="244"/>
+    <row r="21" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A21" s="253"/>
+      <c r="B21" s="244"/>
+      <c r="C21" s="244"/>
+      <c r="D21" s="244"/>
+      <c r="E21" s="244"/>
+      <c r="F21" s="240"/>
+      <c r="G21" s="240"/>
+      <c r="H21" s="240"/>
       <c r="I21" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="J21" s="237"/>
-      <c r="K21" s="238"/>
-      <c r="L21" s="238"/>
+      <c r="J21" s="246"/>
+      <c r="K21" s="244"/>
+      <c r="L21" s="244"/>
       <c r="M21" s="17"/>
     </row>
-    <row r="22" spans="1:13" ht="39" x14ac:dyDescent="0.15">
-      <c r="A22" s="233" t="s">
+    <row r="22" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A22" s="251" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="236"/>
-      <c r="C22" s="236"/>
-      <c r="D22" s="236"/>
-      <c r="E22" s="236"/>
-      <c r="F22" s="242" t="s">
+      <c r="B22" s="243"/>
+      <c r="C22" s="243"/>
+      <c r="D22" s="243"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="239" t="s">
         <v>248</v>
       </c>
-      <c r="G22" s="245">
+      <c r="G22" s="241">
         <v>40695</v>
       </c>
-      <c r="H22" s="245">
+      <c r="H22" s="241">
         <v>40909</v>
       </c>
       <c r="I22" s="23" t="s">
@@ -16145,15 +16158,15 @@
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A23" s="234"/>
-      <c r="B23" s="237"/>
-      <c r="C23" s="237"/>
-      <c r="D23" s="237"/>
-      <c r="E23" s="237"/>
-      <c r="F23" s="243"/>
-      <c r="G23" s="243"/>
-      <c r="H23" s="243"/>
+    <row r="23" spans="1:13" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="252"/>
+      <c r="B23" s="246"/>
+      <c r="C23" s="246"/>
+      <c r="D23" s="246"/>
+      <c r="E23" s="246"/>
+      <c r="F23" s="247"/>
+      <c r="G23" s="247"/>
+      <c r="H23" s="247"/>
       <c r="I23" s="24" t="s">
         <v>321</v>
       </c>
@@ -16162,15 +16175,15 @@
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
     </row>
-    <row r="24" spans="1:13" ht="26" x14ac:dyDescent="0.15">
-      <c r="A24" s="234"/>
-      <c r="B24" s="237"/>
-      <c r="C24" s="237"/>
-      <c r="D24" s="237"/>
-      <c r="E24" s="237"/>
-      <c r="F24" s="243"/>
-      <c r="G24" s="243"/>
-      <c r="H24" s="243"/>
+    <row r="24" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A24" s="252"/>
+      <c r="B24" s="246"/>
+      <c r="C24" s="246"/>
+      <c r="D24" s="246"/>
+      <c r="E24" s="246"/>
+      <c r="F24" s="247"/>
+      <c r="G24" s="247"/>
+      <c r="H24" s="247"/>
       <c r="I24" s="24" t="s">
         <v>331</v>
       </c>
@@ -16179,15 +16192,15 @@
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
     </row>
-    <row r="25" spans="1:13" ht="39" x14ac:dyDescent="0.15">
-      <c r="A25" s="234"/>
-      <c r="B25" s="237"/>
-      <c r="C25" s="237"/>
-      <c r="D25" s="237"/>
-      <c r="E25" s="237"/>
-      <c r="F25" s="243"/>
-      <c r="G25" s="243"/>
-      <c r="H25" s="243"/>
+    <row r="25" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A25" s="252"/>
+      <c r="B25" s="246"/>
+      <c r="C25" s="246"/>
+      <c r="D25" s="246"/>
+      <c r="E25" s="246"/>
+      <c r="F25" s="247"/>
+      <c r="G25" s="247"/>
+      <c r="H25" s="247"/>
       <c r="I25" s="174" t="s">
         <v>411</v>
       </c>
@@ -16196,15 +16209,15 @@
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
     </row>
-    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.15">
-      <c r="A26" s="235"/>
-      <c r="B26" s="238"/>
-      <c r="C26" s="238"/>
-      <c r="D26" s="238"/>
-      <c r="E26" s="238"/>
-      <c r="F26" s="244"/>
-      <c r="G26" s="244"/>
-      <c r="H26" s="244"/>
+    <row r="26" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A26" s="253"/>
+      <c r="B26" s="244"/>
+      <c r="C26" s="244"/>
+      <c r="D26" s="244"/>
+      <c r="E26" s="244"/>
+      <c r="F26" s="240"/>
+      <c r="G26" s="240"/>
+      <c r="H26" s="240"/>
       <c r="I26" s="25" t="s">
         <v>322</v>
       </c>
@@ -16213,107 +16226,107 @@
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
     </row>
-    <row r="27" spans="1:13" ht="78" x14ac:dyDescent="0.15">
-      <c r="A27" s="233" t="s">
+    <row r="27" spans="1:13" ht="84" x14ac:dyDescent="0.15">
+      <c r="A27" s="251" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="236"/>
-      <c r="C27" s="236"/>
-      <c r="D27" s="236"/>
-      <c r="E27" s="236"/>
-      <c r="F27" s="254" t="s">
+      <c r="B27" s="243"/>
+      <c r="C27" s="243"/>
+      <c r="D27" s="243"/>
+      <c r="E27" s="243"/>
+      <c r="F27" s="248" t="s">
         <v>249</v>
       </c>
-      <c r="G27" s="245">
+      <c r="G27" s="241">
         <v>40603</v>
       </c>
-      <c r="H27" s="245">
+      <c r="H27" s="241">
         <v>40664</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="J27" s="237"/>
-      <c r="K27" s="236"/>
-      <c r="L27" s="236"/>
-      <c r="M27" s="236"/>
-    </row>
-    <row r="28" spans="1:13" ht="65" x14ac:dyDescent="0.15">
-      <c r="A28" s="234"/>
-      <c r="B28" s="237"/>
-      <c r="C28" s="237"/>
-      <c r="D28" s="237"/>
-      <c r="E28" s="237"/>
-      <c r="F28" s="255"/>
-      <c r="G28" s="246"/>
-      <c r="H28" s="243"/>
+      <c r="J27" s="246"/>
+      <c r="K27" s="243"/>
+      <c r="L27" s="243"/>
+      <c r="M27" s="243"/>
+    </row>
+    <row r="28" spans="1:13" ht="70" x14ac:dyDescent="0.15">
+      <c r="A28" s="252"/>
+      <c r="B28" s="246"/>
+      <c r="C28" s="246"/>
+      <c r="D28" s="246"/>
+      <c r="E28" s="246"/>
+      <c r="F28" s="249"/>
+      <c r="G28" s="242"/>
+      <c r="H28" s="247"/>
       <c r="I28" s="173" t="s">
         <v>410</v>
       </c>
-      <c r="J28" s="237"/>
-      <c r="K28" s="237"/>
-      <c r="L28" s="237"/>
-      <c r="M28" s="237"/>
-    </row>
-    <row r="29" spans="1:13" ht="39" x14ac:dyDescent="0.15">
-      <c r="A29" s="234"/>
-      <c r="B29" s="238"/>
-      <c r="C29" s="238"/>
-      <c r="D29" s="238"/>
-      <c r="E29" s="238"/>
-      <c r="F29" s="256"/>
-      <c r="G29" s="247"/>
-      <c r="H29" s="244"/>
+      <c r="J28" s="246"/>
+      <c r="K28" s="246"/>
+      <c r="L28" s="246"/>
+      <c r="M28" s="246"/>
+    </row>
+    <row r="29" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A29" s="252"/>
+      <c r="B29" s="244"/>
+      <c r="C29" s="244"/>
+      <c r="D29" s="244"/>
+      <c r="E29" s="244"/>
+      <c r="F29" s="250"/>
+      <c r="G29" s="245"/>
+      <c r="H29" s="240"/>
       <c r="I29" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="J29" s="238"/>
-      <c r="K29" s="238"/>
-      <c r="L29" s="238"/>
-      <c r="M29" s="238"/>
-    </row>
-    <row r="30" spans="1:13" ht="52" x14ac:dyDescent="0.15">
-      <c r="A30" s="234"/>
-      <c r="B30" s="236"/>
-      <c r="C30" s="236"/>
-      <c r="D30" s="236"/>
-      <c r="E30" s="236"/>
-      <c r="F30" s="242" t="s">
+      <c r="J29" s="244"/>
+      <c r="K29" s="244"/>
+      <c r="L29" s="244"/>
+      <c r="M29" s="244"/>
+    </row>
+    <row r="30" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A30" s="252"/>
+      <c r="B30" s="243"/>
+      <c r="C30" s="243"/>
+      <c r="D30" s="243"/>
+      <c r="E30" s="243"/>
+      <c r="F30" s="239" t="s">
         <v>250</v>
       </c>
-      <c r="G30" s="245">
+      <c r="G30" s="241">
         <v>40603</v>
       </c>
-      <c r="H30" s="245">
+      <c r="H30" s="241">
         <v>40664</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="J30" s="236"/>
-      <c r="K30" s="236"/>
-      <c r="L30" s="236"/>
-      <c r="M30" s="236"/>
-    </row>
-    <row r="31" spans="1:13" ht="26" x14ac:dyDescent="0.15">
-      <c r="A31" s="234"/>
-      <c r="B31" s="238"/>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
-      <c r="F31" s="244"/>
-      <c r="G31" s="246"/>
-      <c r="H31" s="244"/>
+      <c r="J30" s="243"/>
+      <c r="K30" s="243"/>
+      <c r="L30" s="243"/>
+      <c r="M30" s="243"/>
+    </row>
+    <row r="31" spans="1:13" ht="28" x14ac:dyDescent="0.15">
+      <c r="A31" s="252"/>
+      <c r="B31" s="244"/>
+      <c r="C31" s="244"/>
+      <c r="D31" s="244"/>
+      <c r="E31" s="244"/>
+      <c r="F31" s="240"/>
+      <c r="G31" s="242"/>
+      <c r="H31" s="240"/>
       <c r="I31" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="J31" s="238"/>
-      <c r="K31" s="238"/>
-      <c r="L31" s="238"/>
-      <c r="M31" s="238"/>
-    </row>
-    <row r="32" spans="1:13" ht="39" x14ac:dyDescent="0.15">
-      <c r="A32" s="234"/>
+      <c r="J31" s="244"/>
+      <c r="K31" s="244"/>
+      <c r="L31" s="244"/>
+      <c r="M31" s="244"/>
+    </row>
+    <row r="32" spans="1:13" ht="42" x14ac:dyDescent="0.15">
+      <c r="A32" s="252"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -16335,45 +16348,45 @@
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
     </row>
-    <row r="33" spans="1:17" ht="39" x14ac:dyDescent="0.15">
-      <c r="A33" s="234"/>
-      <c r="B33" s="236"/>
-      <c r="C33" s="236"/>
-      <c r="D33" s="236"/>
-      <c r="E33" s="236"/>
-      <c r="F33" s="242" t="s">
+    <row r="33" spans="1:17" ht="42" x14ac:dyDescent="0.15">
+      <c r="A33" s="252"/>
+      <c r="B33" s="243"/>
+      <c r="C33" s="243"/>
+      <c r="D33" s="243"/>
+      <c r="E33" s="243"/>
+      <c r="F33" s="239" t="s">
         <v>252</v>
       </c>
-      <c r="G33" s="245">
+      <c r="G33" s="241">
         <v>40603</v>
       </c>
-      <c r="H33" s="245">
+      <c r="H33" s="241">
         <v>40664</v>
       </c>
       <c r="I33" s="172" t="s">
         <v>408</v>
       </c>
-      <c r="J33" s="236"/>
-      <c r="K33" s="236"/>
-      <c r="L33" s="236"/>
-      <c r="M33" s="236"/>
-    </row>
-    <row r="34" spans="1:17" ht="26" x14ac:dyDescent="0.15">
-      <c r="A34" s="235"/>
-      <c r="B34" s="238"/>
-      <c r="C34" s="238"/>
-      <c r="D34" s="238"/>
-      <c r="E34" s="238"/>
-      <c r="F34" s="244"/>
-      <c r="G34" s="247"/>
-      <c r="H34" s="247"/>
+      <c r="J33" s="243"/>
+      <c r="K33" s="243"/>
+      <c r="L33" s="243"/>
+      <c r="M33" s="243"/>
+    </row>
+    <row r="34" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+      <c r="A34" s="253"/>
+      <c r="B34" s="244"/>
+      <c r="C34" s="244"/>
+      <c r="D34" s="244"/>
+      <c r="E34" s="244"/>
+      <c r="F34" s="240"/>
+      <c r="G34" s="245"/>
+      <c r="H34" s="245"/>
       <c r="I34" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="J34" s="238"/>
-      <c r="K34" s="238"/>
-      <c r="L34" s="238"/>
-      <c r="M34" s="238"/>
+      <c r="J34" s="244"/>
+      <c r="K34" s="244"/>
+      <c r="L34" s="244"/>
+      <c r="M34" s="244"/>
     </row>
     <row r="35" spans="1:17" s="70" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="167" t="s">
@@ -16397,21 +16410,21 @@
       <c r="Q35" s="90"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A36" s="261" t="s">
+      <c r="A36" s="234" t="s">
         <v>404</v>
       </c>
-      <c r="B36" s="262"/>
-      <c r="C36" s="262"/>
-      <c r="D36" s="262"/>
-      <c r="E36" s="262"/>
-      <c r="F36" s="262"/>
-      <c r="G36" s="262"/>
-      <c r="H36" s="262"/>
-      <c r="I36" s="262"/>
-      <c r="J36" s="262"/>
-      <c r="K36" s="262"/>
-      <c r="L36" s="262"/>
-      <c r="M36" s="262"/>
+      <c r="B36" s="235"/>
+      <c r="C36" s="235"/>
+      <c r="D36" s="235"/>
+      <c r="E36" s="235"/>
+      <c r="F36" s="235"/>
+      <c r="G36" s="235"/>
+      <c r="H36" s="235"/>
+      <c r="I36" s="235"/>
+      <c r="J36" s="235"/>
+      <c r="K36" s="235"/>
+      <c r="L36" s="235"/>
+      <c r="M36" s="235"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A37" s="212" t="s">
@@ -16431,38 +16444,38 @@
       <c r="M37" s="213"/>
     </row>
     <row r="38" spans="1:17" s="161" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="260" t="s">
+      <c r="A38" s="233" t="s">
         <v>374</v>
       </c>
-      <c r="B38" s="260"/>
-      <c r="C38" s="260"/>
-      <c r="D38" s="260"/>
-      <c r="E38" s="260"/>
-      <c r="F38" s="260"/>
-      <c r="G38" s="260"/>
-      <c r="H38" s="260"/>
-      <c r="I38" s="260"/>
-      <c r="J38" s="260"/>
-      <c r="K38" s="260"/>
-      <c r="L38" s="260"/>
-      <c r="M38" s="260"/>
+      <c r="B38" s="233"/>
+      <c r="C38" s="233"/>
+      <c r="D38" s="233"/>
+      <c r="E38" s="233"/>
+      <c r="F38" s="233"/>
+      <c r="G38" s="233"/>
+      <c r="H38" s="233"/>
+      <c r="I38" s="233"/>
+      <c r="J38" s="233"/>
+      <c r="K38" s="233"/>
+      <c r="L38" s="233"/>
+      <c r="M38" s="233"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A39" s="264" t="s">
+      <c r="A39" s="237" t="s">
         <v>406</v>
       </c>
-      <c r="B39" s="265"/>
-      <c r="C39" s="265"/>
-      <c r="D39" s="265"/>
-      <c r="E39" s="265"/>
-      <c r="F39" s="265"/>
-      <c r="G39" s="265"/>
-      <c r="H39" s="265"/>
-      <c r="I39" s="265"/>
-      <c r="J39" s="265"/>
-      <c r="K39" s="265"/>
-      <c r="L39" s="265"/>
-      <c r="M39" s="265"/>
+      <c r="B39" s="238"/>
+      <c r="C39" s="238"/>
+      <c r="D39" s="238"/>
+      <c r="E39" s="238"/>
+      <c r="F39" s="238"/>
+      <c r="G39" s="238"/>
+      <c r="H39" s="238"/>
+      <c r="I39" s="238"/>
+      <c r="J39" s="238"/>
+      <c r="K39" s="238"/>
+      <c r="L39" s="238"/>
+      <c r="M39" s="238"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A40" s="171" t="s">
@@ -16483,6 +16496,85 @@
     </row>
   </sheetData>
   <mergeCells count="95">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="D4:D9"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="G4:G9"/>
+    <mergeCell ref="H4:H9"/>
+    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="K4:K9"/>
+    <mergeCell ref="L4:L9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="M27:M29"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
     <mergeCell ref="A38:M38"/>
     <mergeCell ref="A37:M37"/>
     <mergeCell ref="A36:M36"/>
@@ -16499,85 +16591,6 @@
     <mergeCell ref="K33:K34"/>
     <mergeCell ref="K27:K29"/>
     <mergeCell ref="L27:L29"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="M27:M29"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="L18:L21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="K10:K13"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="D4:D9"/>
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="F4:F9"/>
-    <mergeCell ref="G4:G9"/>
-    <mergeCell ref="H4:H9"/>
-    <mergeCell ref="J4:J9"/>
-    <mergeCell ref="K4:K9"/>
-    <mergeCell ref="L4:L9"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -16585,8 +16598,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:U94"/>
@@ -16605,26 +16618,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A1" s="263" t="s">
+      <c r="A1" s="236" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="263"/>
-      <c r="J1" s="263"/>
-      <c r="K1" s="263"/>
-      <c r="L1" s="263"/>
-      <c r="M1" s="263"/>
-      <c r="N1" s="263"/>
-      <c r="O1" s="263"/>
-      <c r="P1" s="263"/>
-      <c r="Q1" s="263"/>
-      <c r="R1" s="263"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
+      <c r="N1" s="236"/>
+      <c r="O1" s="236"/>
+      <c r="P1" s="236"/>
+      <c r="Q1" s="236"/>
+      <c r="R1" s="236"/>
     </row>
     <row r="2" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="76"/>
@@ -19577,21 +19590,21 @@
       <c r="Q54" s="90"/>
     </row>
     <row r="55" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="261" t="s">
+      <c r="A55" s="234" t="s">
         <v>404</v>
       </c>
-      <c r="B55" s="262"/>
-      <c r="C55" s="262"/>
-      <c r="D55" s="262"/>
-      <c r="E55" s="262"/>
-      <c r="F55" s="262"/>
-      <c r="G55" s="262"/>
-      <c r="H55" s="262"/>
-      <c r="I55" s="262"/>
-      <c r="J55" s="262"/>
-      <c r="K55" s="262"/>
-      <c r="L55" s="262"/>
-      <c r="M55" s="262"/>
+      <c r="B55" s="235"/>
+      <c r="C55" s="235"/>
+      <c r="D55" s="235"/>
+      <c r="E55" s="235"/>
+      <c r="F55" s="235"/>
+      <c r="G55" s="235"/>
+      <c r="H55" s="235"/>
+      <c r="I55" s="235"/>
+      <c r="J55" s="235"/>
+      <c r="K55" s="235"/>
+      <c r="L55" s="235"/>
+      <c r="M55" s="235"/>
     </row>
     <row r="56" spans="1:18" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="212" t="s">
@@ -19611,26 +19624,26 @@
       <c r="M56" s="213"/>
     </row>
     <row r="57" spans="1:18" s="162" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="260" t="s">
+      <c r="A57" s="233" t="s">
         <v>363</v>
       </c>
-      <c r="B57" s="260"/>
-      <c r="C57" s="260"/>
-      <c r="D57" s="260"/>
-      <c r="E57" s="260"/>
-      <c r="F57" s="260"/>
-      <c r="G57" s="260"/>
-      <c r="H57" s="260"/>
-      <c r="I57" s="260"/>
-      <c r="J57" s="260"/>
-      <c r="K57" s="260"/>
-      <c r="L57" s="260"/>
-      <c r="M57" s="260"/>
-      <c r="N57" s="260"/>
-      <c r="O57" s="260"/>
-      <c r="P57" s="260"/>
-      <c r="Q57" s="260"/>
-      <c r="R57" s="260"/>
+      <c r="B57" s="233"/>
+      <c r="C57" s="233"/>
+      <c r="D57" s="233"/>
+      <c r="E57" s="233"/>
+      <c r="F57" s="233"/>
+      <c r="G57" s="233"/>
+      <c r="H57" s="233"/>
+      <c r="I57" s="233"/>
+      <c r="J57" s="233"/>
+      <c r="K57" s="233"/>
+      <c r="L57" s="233"/>
+      <c r="M57" s="233"/>
+      <c r="N57" s="233"/>
+      <c r="O57" s="233"/>
+      <c r="P57" s="233"/>
+      <c r="Q57" s="233"/>
+      <c r="R57" s="233"/>
     </row>
     <row r="58" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="212" t="s">
@@ -19797,13 +19810,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:AT58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U9" sqref="U9"/>
     </sheetView>
@@ -22778,26 +22791,26 @@
       <c r="R54" s="208"/>
     </row>
     <row r="55" spans="1:46" s="51" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="192" t="s">
+      <c r="A55" s="205" t="s">
         <v>392</v>
       </c>
-      <c r="B55" s="192"/>
-      <c r="C55" s="192"/>
-      <c r="D55" s="192"/>
-      <c r="E55" s="192"/>
-      <c r="F55" s="192"/>
-      <c r="G55" s="192"/>
-      <c r="H55" s="192"/>
-      <c r="I55" s="192"/>
-      <c r="J55" s="192"/>
-      <c r="K55" s="192"/>
-      <c r="L55" s="192"/>
-      <c r="M55" s="192"/>
-      <c r="N55" s="192"/>
-      <c r="O55" s="192"/>
-      <c r="P55" s="192"/>
-      <c r="Q55" s="192"/>
-      <c r="R55" s="192"/>
+      <c r="B55" s="205"/>
+      <c r="C55" s="205"/>
+      <c r="D55" s="205"/>
+      <c r="E55" s="205"/>
+      <c r="F55" s="205"/>
+      <c r="G55" s="205"/>
+      <c r="H55" s="205"/>
+      <c r="I55" s="205"/>
+      <c r="J55" s="205"/>
+      <c r="K55" s="205"/>
+      <c r="L55" s="205"/>
+      <c r="M55" s="205"/>
+      <c r="N55" s="205"/>
+      <c r="O55" s="205"/>
+      <c r="P55" s="205"/>
+      <c r="Q55" s="205"/>
+      <c r="R55" s="205"/>
       <c r="S55" s="62"/>
       <c r="T55" s="62"/>
       <c r="U55" s="62"/>
@@ -22828,26 +22841,26 @@
       <c r="AT55" s="62"/>
     </row>
     <row r="56" spans="1:46" s="51" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="192" t="s">
+      <c r="A56" s="205" t="s">
         <v>337</v>
       </c>
-      <c r="B56" s="192"/>
-      <c r="C56" s="192"/>
-      <c r="D56" s="192"/>
-      <c r="E56" s="192"/>
-      <c r="F56" s="192"/>
-      <c r="G56" s="192"/>
-      <c r="H56" s="192"/>
-      <c r="I56" s="192"/>
-      <c r="J56" s="192"/>
-      <c r="K56" s="192"/>
-      <c r="L56" s="192"/>
-      <c r="M56" s="192"/>
-      <c r="N56" s="192"/>
-      <c r="O56" s="192"/>
-      <c r="P56" s="192"/>
-      <c r="Q56" s="192"/>
-      <c r="R56" s="192"/>
+      <c r="B56" s="205"/>
+      <c r="C56" s="205"/>
+      <c r="D56" s="205"/>
+      <c r="E56" s="205"/>
+      <c r="F56" s="205"/>
+      <c r="G56" s="205"/>
+      <c r="H56" s="205"/>
+      <c r="I56" s="205"/>
+      <c r="J56" s="205"/>
+      <c r="K56" s="205"/>
+      <c r="L56" s="205"/>
+      <c r="M56" s="205"/>
+      <c r="N56" s="205"/>
+      <c r="O56" s="205"/>
+      <c r="P56" s="205"/>
+      <c r="Q56" s="205"/>
+      <c r="R56" s="205"/>
       <c r="S56" s="62"/>
       <c r="T56" s="62"/>
       <c r="U56" s="62"/>
@@ -22928,26 +22941,26 @@
       <c r="AT57" s="62"/>
     </row>
     <row r="58" spans="1:46" s="51" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="192" t="s">
+      <c r="A58" s="205" t="s">
         <v>383</v>
       </c>
-      <c r="B58" s="192"/>
-      <c r="C58" s="192"/>
-      <c r="D58" s="192"/>
-      <c r="E58" s="192"/>
-      <c r="F58" s="192"/>
-      <c r="G58" s="192"/>
-      <c r="H58" s="192"/>
-      <c r="I58" s="192"/>
-      <c r="J58" s="192"/>
-      <c r="K58" s="192"/>
-      <c r="L58" s="192"/>
-      <c r="M58" s="192"/>
-      <c r="N58" s="192"/>
-      <c r="O58" s="192"/>
-      <c r="P58" s="192"/>
-      <c r="Q58" s="192"/>
-      <c r="R58" s="192"/>
+      <c r="B58" s="205"/>
+      <c r="C58" s="205"/>
+      <c r="D58" s="205"/>
+      <c r="E58" s="205"/>
+      <c r="F58" s="205"/>
+      <c r="G58" s="205"/>
+      <c r="H58" s="205"/>
+      <c r="I58" s="205"/>
+      <c r="J58" s="205"/>
+      <c r="K58" s="205"/>
+      <c r="L58" s="205"/>
+      <c r="M58" s="205"/>
+      <c r="N58" s="205"/>
+      <c r="O58" s="205"/>
+      <c r="P58" s="205"/>
+      <c r="Q58" s="205"/>
+      <c r="R58" s="205"/>
       <c r="S58" s="62"/>
       <c r="T58" s="62"/>
       <c r="U58" s="62"/>
@@ -22992,15 +23005,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1:R1048576"/>
+      <selection pane="topRight" activeCell="A57" sqref="A57:R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25973,7 +25986,7 @@
       <c r="R54" s="210"/>
     </row>
     <row r="55" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="192" t="s">
+      <c r="A55" s="205" t="s">
         <v>392</v>
       </c>
       <c r="B55" s="209"/>
@@ -26039,26 +26052,26 @@
       <c r="R57" s="207"/>
     </row>
     <row r="58" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="192" t="s">
+      <c r="A58" s="205" t="s">
         <v>384</v>
       </c>
-      <c r="B58" s="192"/>
-      <c r="C58" s="192"/>
-      <c r="D58" s="192"/>
-      <c r="E58" s="192"/>
-      <c r="F58" s="192"/>
-      <c r="G58" s="192"/>
-      <c r="H58" s="192"/>
-      <c r="I58" s="192"/>
-      <c r="J58" s="192"/>
-      <c r="K58" s="192"/>
-      <c r="L58" s="192"/>
-      <c r="M58" s="192"/>
-      <c r="N58" s="192"/>
-      <c r="O58" s="192"/>
-      <c r="P58" s="192"/>
-      <c r="Q58" s="192"/>
-      <c r="R58" s="192"/>
+      <c r="B58" s="205"/>
+      <c r="C58" s="205"/>
+      <c r="D58" s="205"/>
+      <c r="E58" s="205"/>
+      <c r="F58" s="205"/>
+      <c r="G58" s="205"/>
+      <c r="H58" s="205"/>
+      <c r="I58" s="205"/>
+      <c r="J58" s="205"/>
+      <c r="K58" s="205"/>
+      <c r="L58" s="205"/>
+      <c r="M58" s="205"/>
+      <c r="N58" s="205"/>
+      <c r="O58" s="205"/>
+      <c r="P58" s="205"/>
+      <c r="Q58" s="205"/>
+      <c r="R58" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -26076,15 +26089,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1:R1048576"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -29130,8 +29143,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:R60"/>
@@ -29161,7 +29174,7 @@
       <c r="G1" s="217"/>
       <c r="H1" s="217"/>
     </row>
-    <row r="2" spans="1:8" ht="39" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="76"/>
       <c r="B2" s="71">
         <v>2009</v>
@@ -30550,14 +30563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U9" sqref="U9"/>
     </sheetView>
@@ -33659,8 +33672,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:AO64"/>
@@ -33783,7 +33796,7 @@
       <c r="AN2" s="223"/>
       <c r="AO2" s="223"/>
     </row>
-    <row r="3" spans="1:41" s="79" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:41" s="79" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="225"/>
       <c r="B3" s="100" t="s">
         <v>163</v>
@@ -33896,7 +33909,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="52" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="107" t="s">
         <v>0</v>
       </c>
@@ -33998,7 +34011,7 @@
       <c r="AN5" s="117"/>
       <c r="AO5" s="118"/>
     </row>
-    <row r="6" spans="1:41" ht="65" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="88" t="s">
         <v>2</v>
       </c>
@@ -34145,7 +34158,7 @@
       <c r="AN8" s="117"/>
       <c r="AO8" s="118"/>
     </row>
-    <row r="9" spans="1:41" ht="78" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:41" ht="84" x14ac:dyDescent="0.15">
       <c r="A9" s="226" t="s">
         <v>5</v>
       </c>
@@ -34196,7 +34209,7 @@
       <c r="AN9" s="126"/>
       <c r="AO9" s="127"/>
     </row>
-    <row r="10" spans="1:41" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:41" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="228"/>
       <c r="B10" s="95"/>
       <c r="C10" s="89"/>
@@ -34386,7 +34399,7 @@
       <c r="AN13" s="117"/>
       <c r="AO13" s="118"/>
     </row>
-    <row r="14" spans="1:41" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:41" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="88" t="s">
         <v>8</v>
       </c>
@@ -34437,7 +34450,7 @@
       <c r="AN14" s="117"/>
       <c r="AO14" s="118"/>
     </row>
-    <row r="15" spans="1:41" ht="39" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:41" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" s="226" t="s">
         <v>9</v>
       </c>
@@ -34488,7 +34501,7 @@
       <c r="AN15" s="126"/>
       <c r="AO15" s="127"/>
     </row>
-    <row r="16" spans="1:41" ht="143" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:41" ht="154" x14ac:dyDescent="0.15">
       <c r="A16" s="228"/>
       <c r="B16" s="95"/>
       <c r="C16" s="89"/>
@@ -34612,7 +34625,7 @@
       <c r="AN17" s="117"/>
       <c r="AO17" s="118"/>
     </row>
-    <row r="18" spans="1:41" ht="143" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:41" ht="154" x14ac:dyDescent="0.15">
       <c r="A18" s="88" t="s">
         <v>11</v>
       </c>
@@ -34714,7 +34727,7 @@
       <c r="AN19" s="117"/>
       <c r="AO19" s="118"/>
     </row>
-    <row r="20" spans="1:41" ht="65" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:41" ht="70" x14ac:dyDescent="0.15">
       <c r="A20" s="88" t="s">
         <v>13</v>
       </c>
@@ -34906,7 +34919,7 @@
       <c r="AN23" s="117"/>
       <c r="AO23" s="118"/>
     </row>
-    <row r="24" spans="1:41" ht="39" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:41" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="226" t="s">
         <v>17</v>
       </c>
@@ -34963,7 +34976,7 @@
       <c r="AN24" s="126"/>
       <c r="AO24" s="137"/>
     </row>
-    <row r="25" spans="1:41" ht="52" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:41" ht="70" x14ac:dyDescent="0.15">
       <c r="A25" s="227"/>
       <c r="B25" s="95"/>
       <c r="C25" s="89"/>
@@ -35147,7 +35160,7 @@
       <c r="AN28" s="117"/>
       <c r="AO28" s="118"/>
     </row>
-    <row r="29" spans="1:41" ht="39" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:41" ht="42" x14ac:dyDescent="0.15">
       <c r="A29" s="88" t="s">
         <v>48</v>
       </c>
@@ -35198,7 +35211,7 @@
       <c r="AN29" s="117"/>
       <c r="AO29" s="118"/>
     </row>
-    <row r="30" spans="1:41" ht="39" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:41" ht="42" x14ac:dyDescent="0.15">
       <c r="A30" s="88"/>
       <c r="B30" s="95"/>
       <c r="C30" s="89"/>
@@ -35247,7 +35260,7 @@
       <c r="AN30" s="126"/>
       <c r="AO30" s="127"/>
     </row>
-    <row r="31" spans="1:41" ht="117" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:41" ht="140" x14ac:dyDescent="0.15">
       <c r="A31" s="88" t="s">
         <v>21</v>
       </c>
@@ -35304,7 +35317,7 @@
       <c r="AN31" s="132"/>
       <c r="AO31" s="133"/>
     </row>
-    <row r="32" spans="1:41" ht="65" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:41" ht="70" x14ac:dyDescent="0.15">
       <c r="A32" s="88" t="s">
         <v>22</v>
       </c>
@@ -35355,7 +35368,7 @@
       <c r="AN32" s="117"/>
       <c r="AO32" s="118"/>
     </row>
-    <row r="33" spans="1:41" ht="65" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:41" ht="70" x14ac:dyDescent="0.15">
       <c r="A33" s="88" t="s">
         <v>23</v>
       </c>
@@ -35457,7 +35470,7 @@
       <c r="AN34" s="117"/>
       <c r="AO34" s="118"/>
     </row>
-    <row r="35" spans="1:41" ht="78" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:41" ht="84" x14ac:dyDescent="0.15">
       <c r="A35" s="88" t="s">
         <v>25</v>
       </c>
@@ -35553,7 +35566,7 @@
       <c r="AN36" s="117"/>
       <c r="AO36" s="118"/>
     </row>
-    <row r="37" spans="1:41" ht="52" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:41" ht="56" x14ac:dyDescent="0.15">
       <c r="A37" s="88" t="s">
         <v>27</v>
       </c>
@@ -35739,7 +35752,7 @@
       <c r="AN40" s="117"/>
       <c r="AO40" s="118"/>
     </row>
-    <row r="41" spans="1:41" ht="182" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:41" ht="196" x14ac:dyDescent="0.15">
       <c r="A41" s="88" t="s">
         <v>31</v>
       </c>
@@ -35898,7 +35911,7 @@
       <c r="AN43" s="117"/>
       <c r="AO43" s="118"/>
     </row>
-    <row r="44" spans="1:41" ht="91" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:41" ht="112" x14ac:dyDescent="0.15">
       <c r="A44" s="88" t="s">
         <v>34</v>
       </c>
@@ -35994,7 +36007,7 @@
       <c r="AN45" s="117"/>
       <c r="AO45" s="118"/>
     </row>
-    <row r="46" spans="1:41" ht="26" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:41" ht="28" x14ac:dyDescent="0.15">
       <c r="A46" s="88" t="s">
         <v>36</v>
       </c>
@@ -36045,7 +36058,7 @@
       <c r="AN46" s="117"/>
       <c r="AO46" s="118"/>
     </row>
-    <row r="47" spans="1:41" ht="78" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:41" ht="84" x14ac:dyDescent="0.15">
       <c r="A47" s="88" t="s">
         <v>37</v>
       </c>
@@ -36210,7 +36223,7 @@
       <c r="AN49" s="117"/>
       <c r="AO49" s="118"/>
     </row>
-    <row r="50" spans="1:41" ht="65" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:41" ht="70" x14ac:dyDescent="0.15">
       <c r="A50" s="88" t="s">
         <v>39</v>
       </c>
@@ -36432,7 +36445,7 @@
       <c r="AN53" s="117"/>
       <c r="AO53" s="118"/>
     </row>
-    <row r="54" spans="1:41" ht="52" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:41" ht="56" x14ac:dyDescent="0.15">
       <c r="A54" s="88" t="s">
         <v>43</v>
       </c>
@@ -36534,7 +36547,7 @@
       <c r="AN55" s="117"/>
       <c r="AO55" s="118"/>
     </row>
-    <row r="56" spans="1:41" ht="26" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:41" ht="28" x14ac:dyDescent="0.15">
       <c r="A56" s="88" t="s">
         <v>45</v>
       </c>
@@ -36826,8 +36839,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:U59"/>
@@ -39881,8 +39894,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:AO61"/>
@@ -39999,7 +40012,7 @@
       <c r="AN2" s="223"/>
       <c r="AO2" s="223"/>
     </row>
-    <row r="3" spans="1:41" s="79" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:41" s="79" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="151"/>
       <c r="B3" s="100" t="s">
         <v>163</v>
@@ -40292,7 +40305,7 @@
       <c r="AN7" s="114"/>
       <c r="AO7" s="115"/>
     </row>
-    <row r="8" spans="1:41" ht="78" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:41" ht="84" x14ac:dyDescent="0.15">
       <c r="A8" s="152" t="s">
         <v>4</v>
       </c>
@@ -40703,7 +40716,7 @@
       <c r="AN16" s="114"/>
       <c r="AO16" s="115"/>
     </row>
-    <row r="17" spans="1:41" ht="65" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:41" ht="70" x14ac:dyDescent="0.15">
       <c r="A17" s="226" t="s">
         <v>12</v>
       </c>
@@ -40760,7 +40773,7 @@
       <c r="AN17" s="126"/>
       <c r="AO17" s="129"/>
     </row>
-    <row r="18" spans="1:41" ht="78" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:41" ht="84" x14ac:dyDescent="0.15">
       <c r="A18" s="228"/>
       <c r="B18" s="95"/>
       <c r="C18" s="89"/>

</xml_diff>